<commit_message>
update SRS According to CSR IN RTM
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\ProjectManagement\project\Learning-hub\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -368,25 +368,10 @@
     <t>Lhub_SRS_2.4.3.11</t>
   </si>
   <si>
-    <t>Lhub_SRS_2.4.4.12</t>
-  </si>
-  <si>
     <t>Lhub_SRS_2.4.4.1
 Lhub_SRS_2.4.4.2</t>
   </si>
   <si>
-    <t>Lhub_SRS_2.4.4.13</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.4.14</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.4.15</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.3.15</t>
-  </si>
-  <si>
     <t>Lhub_SRS_2.4.2.14</t>
   </si>
   <si>
@@ -409,6 +394,21 @@
   </si>
   <si>
     <t xml:space="preserve">update the SRS IDs column according to SRS document </t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.4</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.5</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.6</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.12</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.13</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -761,9 +761,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,9 +770,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -785,46 +779,106 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -839,34 +893,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -889,33 +919,6 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1242,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="17.399999999999999"/>
@@ -1265,29 +1268,29 @@
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="48"/>
+      <c r="D1" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="73"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="13" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>52</v>
@@ -1297,13 +1300,13 @@
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="73"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="14">
         <v>1</v>
       </c>
@@ -1311,23 +1314,23 @@
         <v>43588</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="47" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="74">
+      <c r="A4" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="84">
         <v>43470</v>
       </c>
-      <c r="C4" s="74"/>
+      <c r="C4" s="84"/>
       <c r="D4" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -1335,34 +1338,34 @@
         <v>43592</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="47" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="14">
         <v>1.2</v>
       </c>
       <c r="E5" s="15">
         <v>43601</v>
       </c>
-      <c r="F5" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="50"/>
-    </row>
-    <row r="6" spans="1:26" s="49" customFormat="1" ht="93" customHeight="1">
+      <c r="F5" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:26" s="46" customFormat="1" ht="93" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -1389,22 +1392,22 @@
       </c>
     </row>
     <row r="7" spans="1:26" s="4" customFormat="1" ht="37.799999999999997" customHeight="1">
-      <c r="A7" s="76">
+      <c r="A7" s="64">
         <v>1</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="31" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="78"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="78"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1425,18 +1428,18 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A8" s="76"/>
-      <c r="B8" s="75"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="31" t="s">
+      <c r="D8" s="65"/>
+      <c r="E8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="78"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="78"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="67"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1485,24 +1488,24 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="18" customHeight="1">
-      <c r="A10" s="76">
+      <c r="A10" s="64">
         <v>2</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="63" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="31" t="s">
+      <c r="D10" s="65"/>
+      <c r="E10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="79" t="s">
+      <c r="F10" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="41"/>
-      <c r="H10" s="76"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="64"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1523,18 +1526,18 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A11" s="76"/>
-      <c r="B11" s="75"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="31" t="s">
+      <c r="D11" s="65"/>
+      <c r="E11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="76"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="64"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1555,18 +1558,18 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="76"/>
-      <c r="B12" s="75"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="31" t="s">
+      <c r="D12" s="65"/>
+      <c r="E12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="80"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1587,18 +1590,18 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="76"/>
-      <c r="B13" s="75"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="77"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="65"/>
+      <c r="E13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="80"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1619,18 +1622,18 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="76"/>
-      <c r="B14" s="75"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="31" t="s">
+      <c r="D14" s="65"/>
+      <c r="E14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="80"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1651,16 +1654,16 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="76"/>
-      <c r="B15" s="75"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="24"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="31" t="s">
+      <c r="D15" s="65"/>
+      <c r="E15" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1681,16 +1684,16 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="76"/>
-      <c r="B16" s="75"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="31" t="s">
+      <c r="D16" s="65"/>
+      <c r="E16" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="80"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1711,16 +1714,16 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="76"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="31" t="s">
+      <c r="D17" s="65"/>
+      <c r="E17" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="80"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1741,16 +1744,16 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="76"/>
-      <c r="B18" s="75"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="31" t="s">
+      <c r="D18" s="65"/>
+      <c r="E18" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="80"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1771,16 +1774,16 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="76"/>
-      <c r="B19" s="75"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="24"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="31" t="s">
+      <c r="D19" s="65"/>
+      <c r="E19" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="80"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1801,16 +1804,16 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="76"/>
-      <c r="B20" s="75"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="24"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="31" t="s">
+      <c r="D20" s="65"/>
+      <c r="E20" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="80"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1831,16 +1834,16 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="76"/>
-      <c r="B21" s="75"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="24"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="31" t="s">
+      <c r="D21" s="65"/>
+      <c r="E21" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="80"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1861,16 +1864,16 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="76"/>
-      <c r="B22" s="75"/>
+      <c r="A22" s="64"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="24"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="31" t="s">
+      <c r="D22" s="65"/>
+      <c r="E22" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1891,16 +1894,16 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="76"/>
-      <c r="B23" s="75"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="31" t="s">
+      <c r="D23" s="65"/>
+      <c r="E23" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="80"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1921,16 +1924,16 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="76"/>
-      <c r="B24" s="75"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="31" t="s">
+      <c r="D24" s="65"/>
+      <c r="E24" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="80"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1951,16 +1954,16 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="76"/>
-      <c r="B25" s="75"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="31" t="s">
+      <c r="D25" s="65"/>
+      <c r="E25" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="80"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1981,16 +1984,16 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="76"/>
-      <c r="B26" s="75"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="31" t="s">
+      <c r="D26" s="65"/>
+      <c r="E26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="80"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2011,16 +2014,16 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="76"/>
-      <c r="B27" s="75"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="24"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="31" t="s">
+      <c r="D27" s="65"/>
+      <c r="E27" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="80"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2041,16 +2044,16 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="76"/>
-      <c r="B28" s="75"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="31" t="s">
+      <c r="D28" s="65"/>
+      <c r="E28" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="80"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2075,12 +2078,12 @@
       <c r="B29" s="20"/>
       <c r="C29" s="22"/>
       <c r="D29" s="27"/>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2105,12 +2108,12 @@
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
       <c r="D30" s="27"/>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2135,12 +2138,12 @@
       <c r="B31" s="20"/>
       <c r="C31" s="22"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2165,12 +2168,12 @@
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2195,12 +2198,12 @@
       <c r="B33" s="20"/>
       <c r="C33" s="22"/>
       <c r="D33" s="27"/>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2225,12 +2228,12 @@
       <c r="B34" s="20"/>
       <c r="C34" s="22"/>
       <c r="D34" s="27"/>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2255,12 +2258,12 @@
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
       <c r="D35" s="27"/>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2285,12 +2288,12 @@
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
       <c r="D36" s="27"/>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="42"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="39"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2315,12 +2318,12 @@
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
       <c r="D37" s="27"/>
-      <c r="E37" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="42"/>
+      <c r="E37" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="34"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="39"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2346,9 +2349,9 @@
       <c r="C38" s="23"/>
       <c r="D38" s="26"/>
       <c r="E38" s="19"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="46"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="43"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -2379,14 +2382,14 @@
         <v>17</v>
       </c>
       <c r="D39" s="28"/>
-      <c r="E39" s="32" t="s">
+      <c r="E39" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="56" t="s">
+      <c r="F39" s="54" t="s">
         <v>92</v>
       </c>
       <c r="G39" s="12"/>
-      <c r="H39" s="42"/>
+      <c r="H39" s="39"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2413,12 +2416,12 @@
         <v>18</v>
       </c>
       <c r="D40" s="28"/>
-      <c r="E40" s="32" t="s">
+      <c r="E40" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="57"/>
+      <c r="F40" s="74"/>
       <c r="G40" s="12"/>
-      <c r="H40" s="42"/>
+      <c r="H40" s="39"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2445,12 +2448,12 @@
         <v>19</v>
       </c>
       <c r="D41" s="28"/>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="57"/>
+      <c r="F41" s="74"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="42"/>
+      <c r="H41" s="39"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2475,10 +2478,12 @@
       <c r="B42" s="20"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="57"/>
+      <c r="E42" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="74"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="42"/>
+      <c r="H42" s="39"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2505,12 +2510,12 @@
         <v>20</v>
       </c>
       <c r="D43" s="22"/>
-      <c r="E43" s="32" t="s">
+      <c r="E43" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="58"/>
+      <c r="F43" s="75"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="42"/>
+      <c r="H43" s="39"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2537,12 +2542,12 @@
         <v>88</v>
       </c>
       <c r="D44" s="22"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="36" t="s">
+      <c r="E44" s="31"/>
+      <c r="F44" s="34" t="s">
         <v>82</v>
       </c>
       <c r="G44" s="12"/>
-      <c r="H44" s="42"/>
+      <c r="H44" s="39"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2568,9 +2573,9 @@
       <c r="C45" s="23"/>
       <c r="D45" s="26"/>
       <c r="E45" s="19"/>
-      <c r="F45" s="37"/>
+      <c r="F45" s="35"/>
       <c r="G45" s="17"/>
-      <c r="H45" s="46"/>
+      <c r="H45" s="43"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -2591,26 +2596,26 @@
       <c r="Z45" s="6"/>
     </row>
     <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A46" s="59">
+      <c r="A46" s="57">
         <v>4</v>
       </c>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="60" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="F46" s="56" t="s">
+      <c r="D46" s="66"/>
+      <c r="E46" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="G46" s="42" t="s">
+      <c r="G46" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="H46" s="42"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -2631,18 +2636,18 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A47" s="60"/>
-      <c r="B47" s="63"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="61"/>
       <c r="C47" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="66"/>
-      <c r="E47" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="F47" s="57"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" s="74"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -2663,16 +2668,16 @@
       <c r="Z47" s="9"/>
     </row>
     <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A48" s="60"/>
-      <c r="B48" s="63"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="61"/>
       <c r="C48" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="66"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -2693,14 +2698,14 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="66"/>
-      <c r="E49" s="71"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2721,14 +2726,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="61"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
+      <c r="A50" s="59"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="77"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2754,9 +2759,9 @@
       <c r="C51" s="23"/>
       <c r="D51" s="26"/>
       <c r="E51" s="19"/>
-      <c r="F51" s="37"/>
+      <c r="F51" s="35"/>
       <c r="G51" s="17"/>
-      <c r="H51" s="46"/>
+      <c r="H51" s="43"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -2777,24 +2782,24 @@
       <c r="Z51" s="6"/>
     </row>
     <row r="52" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A52" s="76">
+      <c r="A52" s="64">
         <v>5</v>
       </c>
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="63" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="28"/>
-      <c r="E52" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F52" s="56" t="s">
+      <c r="E52" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" s="54" t="s">
         <v>94</v>
       </c>
       <c r="G52" s="12"/>
-      <c r="H52" s="42"/>
+      <c r="H52" s="39"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2815,16 +2820,16 @@
       <c r="Z52" s="3"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A53" s="76"/>
-      <c r="B53" s="75"/>
+      <c r="A53" s="64"/>
+      <c r="B53" s="63"/>
       <c r="C53" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="28"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="81"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="42"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="39"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2845,16 +2850,16 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="76"/>
-      <c r="B54" s="75"/>
+      <c r="A54" s="64"/>
+      <c r="B54" s="63"/>
       <c r="C54" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D54" s="28"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="82"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="56"/>
       <c r="G54" s="12"/>
-      <c r="H54" s="42"/>
+      <c r="H54" s="39"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2880,9 +2885,9 @@
       <c r="C55" s="23"/>
       <c r="D55" s="26"/>
       <c r="E55" s="19"/>
-      <c r="F55" s="37"/>
+      <c r="F55" s="35"/>
       <c r="G55" s="17"/>
-      <c r="H55" s="46"/>
+      <c r="H55" s="43"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -2903,24 +2908,22 @@
       <c r="Z55" s="6"/>
     </row>
     <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="76">
+      <c r="A56" s="64">
         <v>6</v>
       </c>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56" s="77"/>
-      <c r="E56" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F56" s="56" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F56" s="54" t="s">
         <v>96</v>
       </c>
       <c r="G56" s="12"/>
-      <c r="H56" s="42"/>
+      <c r="H56" s="39"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -2941,16 +2944,15 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A57" s="76"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="F57" s="81"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="42"/>
+      <c r="A57" s="64"/>
+      <c r="B57" s="63"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="55"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="39"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2971,16 +2973,18 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A58" s="76"/>
-      <c r="B58" s="75"/>
-      <c r="C58" s="83"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F58" s="82"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="42"/>
+      <c r="A58" s="64"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="66"/>
+      <c r="E58" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" s="56"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="39"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3001,16 +3005,16 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A59" s="12"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="22"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="53"/>
       <c r="D59" s="29"/>
-      <c r="E59" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="F59" s="38"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="42"/>
+      <c r="E59" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F59" s="52"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="39"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3031,16 +3035,16 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A60" s="12"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="F60" s="38"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="42"/>
+      <c r="A60" s="50"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" s="52"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="39"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3060,149 +3064,151 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A61" s="12"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F61" s="38"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-      <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
-      <c r="X61" s="3"/>
-      <c r="Y61" s="3"/>
-      <c r="Z61" s="3"/>
-    </row>
-    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.8" customHeight="1">
-      <c r="A62" s="17"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
-      <c r="N62" s="6"/>
-      <c r="O62" s="6"/>
-      <c r="P62" s="6"/>
-      <c r="Q62" s="6"/>
-      <c r="R62" s="6"/>
-      <c r="S62" s="6"/>
-      <c r="T62" s="6"/>
-      <c r="U62" s="6"/>
-      <c r="V62" s="6"/>
-      <c r="W62" s="6"/>
-      <c r="X62" s="6"/>
-      <c r="Y62" s="6"/>
-      <c r="Z62" s="6"/>
-    </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.8" customHeight="1">
-      <c r="A63" s="12">
+    <row r="61" spans="1:26" s="7" customFormat="1" ht="22.8" customHeight="1">
+      <c r="A61" s="17"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+      <c r="W61" s="6"/>
+      <c r="X61" s="6"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="6"/>
+    </row>
+    <row r="62" spans="1:26" s="4" customFormat="1" ht="67.8" customHeight="1">
+      <c r="A62" s="12">
         <v>7</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B62" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C62" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="27"/>
-      <c r="E63" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="F63" s="39" t="s">
+      <c r="D62" s="27"/>
+      <c r="E62" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F62" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="G63" s="45"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-      <c r="Q63" s="3"/>
-      <c r="R63" s="3"/>
-      <c r="S63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-      <c r="V63" s="3"/>
-      <c r="W63" s="3"/>
-      <c r="X63" s="3"/>
-      <c r="Y63" s="3"/>
-      <c r="Z63" s="3"/>
-    </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
-      <c r="A64" s="17"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
-      <c r="N64" s="6"/>
-      <c r="O64" s="6"/>
-      <c r="P64" s="6"/>
-      <c r="Q64" s="6"/>
-      <c r="R64" s="6"/>
-      <c r="S64" s="6"/>
-      <c r="T64" s="6"/>
-      <c r="U64" s="6"/>
-      <c r="V64" s="6"/>
-      <c r="W64" s="6"/>
-      <c r="X64" s="6"/>
-      <c r="Y64" s="6"/>
-      <c r="Z64" s="6"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3"/>
+    </row>
+    <row r="63" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
+      <c r="A63" s="17"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="6"/>
+      <c r="T63" s="6"/>
+      <c r="U63" s="6"/>
+      <c r="V63" s="6"/>
+      <c r="W63" s="6"/>
+      <c r="X63" s="6"/>
+      <c r="Y63" s="6"/>
+      <c r="Z63" s="6"/>
+    </row>
+    <row r="64" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A64" s="57">
+        <v>8</v>
+      </c>
+      <c r="B64" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F64" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="G64" s="42"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
+      <c r="X64" s="3"/>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="3"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="59">
-        <v>8</v>
-      </c>
-      <c r="B65" s="62" t="s">
-        <v>37</v>
-      </c>
+      <c r="A65" s="58"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D65" s="27"/>
       <c r="E65" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="F65" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="G65" s="45"/>
-      <c r="H65" s="42"/>
+        <v>78</v>
+      </c>
+      <c r="F65" s="55"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="39"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3223,18 +3229,18 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="60"/>
-      <c r="B66" s="63"/>
+      <c r="A66" s="58"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D66" s="27"/>
       <c r="E66" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F66" s="81"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="42"/>
+        <v>79</v>
+      </c>
+      <c r="F66" s="55"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="39"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -3255,18 +3261,14 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="60"/>
-      <c r="B67" s="63"/>
-      <c r="C67" s="22" t="s">
-        <v>85</v>
-      </c>
+      <c r="A67" s="59"/>
+      <c r="B67" s="62"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="27"/>
-      <c r="E67" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F67" s="81"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="56"/>
       <c r="G67" s="12"/>
-      <c r="H67" s="42"/>
+      <c r="H67" s="39"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -3286,117 +3288,72 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="61"/>
-      <c r="B68" s="64"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="82"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
-      <c r="O68" s="3"/>
-      <c r="P68" s="3"/>
-      <c r="Q68" s="3"/>
-      <c r="R68" s="3"/>
-      <c r="S68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
-      <c r="X68" s="3"/>
-      <c r="Y68" s="3"/>
-      <c r="Z68" s="3"/>
-    </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
-      <c r="A69" s="17"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="46"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
-      <c r="S69" s="6"/>
-      <c r="T69" s="6"/>
-      <c r="U69" s="6"/>
-      <c r="V69" s="6"/>
-      <c r="W69" s="6"/>
-      <c r="X69" s="6"/>
-      <c r="Y69" s="6"/>
-      <c r="Z69" s="6"/>
-    </row>
-    <row r="70" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A70" s="12">
+    <row r="68" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+      <c r="A68" s="17"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="6"/>
+      <c r="W68" s="6"/>
+      <c r="X68" s="6"/>
+      <c r="Y68" s="6"/>
+      <c r="Z68" s="6"/>
+    </row>
+    <row r="69" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A69" s="12">
         <v>9</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B69" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C70" s="22"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="F70" s="39" t="s">
+      <c r="C69" s="22"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="G70" s="12"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="3"/>
-      <c r="P70" s="3"/>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
-      <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
-      <c r="V70" s="3"/>
-      <c r="W70" s="3"/>
-      <c r="X70" s="3"/>
-      <c r="Y70" s="3"/>
-      <c r="Z70" s="3"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
+      <c r="V69" s="3"/>
+      <c r="W69" s="3"/>
+      <c r="X69" s="3"/>
+      <c r="Y69" s="3"/>
+      <c r="Z69" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A10:A28"/>
-    <mergeCell ref="D10:D28"/>
-    <mergeCell ref="F10:F28"/>
+  <mergeCells count="32">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F46:F50"/>
@@ -3413,6 +3370,22 @@
     <mergeCell ref="B10:B28"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A10:A28"/>
+    <mergeCell ref="D10:D28"/>
+    <mergeCell ref="F10:F28"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
   </mergeCells>
   <conditionalFormatting sqref="B6">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
write that wafaa review trm
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
   <si>
     <t>Project Name:</t>
   </si>
@@ -686,7 +686,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -833,14 +833,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,43 +872,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -918,6 +894,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1245,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z69"/>
+  <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="17.399999999999999"/>
@@ -1268,21 +1274,21 @@
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="13" t="s">
         <v>51</v>
       </c>
@@ -1303,10 +1309,10 @@
       <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="14">
         <v>1</v>
       </c>
@@ -1327,10 +1333,10 @@
       <c r="A4" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="84">
+      <c r="B4" s="76">
         <v>43470</v>
       </c>
-      <c r="C4" s="84"/>
+      <c r="C4" s="76"/>
       <c r="D4" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -1349,8 +1355,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="44"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="14">
         <v>1.2</v>
       </c>
@@ -1363,83 +1369,63 @@
       <c r="G5" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="47"/>
-    </row>
-    <row r="6" spans="1:26" s="46" customFormat="1" ht="93" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="H5" s="47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A6" s="44"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="93" customHeight="1">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="4" customFormat="1" ht="37.799999999999997" customHeight="1">
-      <c r="A7" s="64">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.799999999999997" customHeight="1">
+      <c r="A8" s="78">
         <v>1</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B8" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="30" t="s">
+      <c r="D8" s="79"/>
+      <c r="E8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="67"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="67"/>
+      <c r="H8" s="80"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1459,85 +1445,85 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="13.8" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" s="4" customFormat="1" ht="18" customHeight="1">
-      <c r="A10" s="64">
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A9" s="78"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="79"/>
+      <c r="E9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="80"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.8" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="18" customHeight="1">
+      <c r="A11" s="78">
         <v>2</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B11" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="30" t="s">
+      <c r="D11" s="79"/>
+      <c r="E11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="F11" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A11" s="64"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="64"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1557,19 +1543,19 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="64"/>
-      <c r="B12" s="63"/>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A12" s="78"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="65"/>
+        <v>15</v>
+      </c>
+      <c r="D12" s="79"/>
       <c r="E12" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="69"/>
+        <v>39</v>
+      </c>
+      <c r="F12" s="82"/>
       <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1590,16 +1576,16 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="64"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="65"/>
+        <v>16</v>
+      </c>
+      <c r="D13" s="79"/>
       <c r="E13" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="69"/>
+        <v>40</v>
+      </c>
+      <c r="F13" s="82"/>
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
       <c r="I13" s="3"/>
@@ -1622,16 +1608,16 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="64"/>
-      <c r="B14" s="63"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="65"/>
+        <v>87</v>
+      </c>
+      <c r="D14" s="79"/>
       <c r="E14" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="69"/>
+        <v>41</v>
+      </c>
+      <c r="F14" s="82"/>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
       <c r="I14" s="3"/>
@@ -1654,14 +1640,16 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="64"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="65"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="79"/>
       <c r="E15" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="69"/>
+        <v>42</v>
+      </c>
+      <c r="F15" s="82"/>
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
       <c r="I15" s="3"/>
@@ -1684,14 +1672,14 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="64"/>
-      <c r="B16" s="63"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="65"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="69"/>
+        <v>56</v>
+      </c>
+      <c r="F16" s="82"/>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="3"/>
@@ -1714,14 +1702,14 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="65"/>
+      <c r="D17" s="79"/>
       <c r="E17" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="69"/>
+        <v>57</v>
+      </c>
+      <c r="F17" s="82"/>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
       <c r="I17" s="3"/>
@@ -1744,14 +1732,14 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="64"/>
-      <c r="B18" s="63"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="65"/>
+      <c r="D18" s="79"/>
       <c r="E18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="69"/>
+        <v>58</v>
+      </c>
+      <c r="F18" s="82"/>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
       <c r="I18" s="3"/>
@@ -1774,14 +1762,14 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="64"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="24"/>
-      <c r="D19" s="65"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="69"/>
+        <v>59</v>
+      </c>
+      <c r="F19" s="82"/>
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
       <c r="I19" s="3"/>
@@ -1804,14 +1792,14 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="64"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="24"/>
-      <c r="D20" s="65"/>
+      <c r="D20" s="79"/>
       <c r="E20" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="69"/>
+        <v>60</v>
+      </c>
+      <c r="F20" s="82"/>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
       <c r="I20" s="3"/>
@@ -1834,14 +1822,14 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="64"/>
-      <c r="B21" s="63"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="24"/>
-      <c r="D21" s="65"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="F21" s="82"/>
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
       <c r="I21" s="3"/>
@@ -1864,14 +1852,14 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="64"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="24"/>
-      <c r="D22" s="65"/>
+      <c r="D22" s="79"/>
       <c r="E22" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="69"/>
+        <v>62</v>
+      </c>
+      <c r="F22" s="82"/>
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
       <c r="I22" s="3"/>
@@ -1894,14 +1882,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="64"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="65"/>
+      <c r="D23" s="79"/>
       <c r="E23" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="69"/>
+        <v>63</v>
+      </c>
+      <c r="F23" s="82"/>
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
       <c r="I23" s="3"/>
@@ -1924,14 +1912,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="64"/>
-      <c r="B24" s="63"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="65"/>
+      <c r="D24" s="79"/>
       <c r="E24" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="69"/>
+        <v>64</v>
+      </c>
+      <c r="F24" s="82"/>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
       <c r="I24" s="3"/>
@@ -1954,14 +1942,14 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="64"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="65"/>
+      <c r="D25" s="79"/>
       <c r="E25" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="F25" s="82"/>
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
       <c r="I25" s="3"/>
@@ -1984,14 +1972,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="64"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="65"/>
+      <c r="D26" s="79"/>
       <c r="E26" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="69"/>
+        <v>44</v>
+      </c>
+      <c r="F26" s="82"/>
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
       <c r="I26" s="3"/>
@@ -2014,14 +2002,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="64"/>
-      <c r="B27" s="63"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="24"/>
-      <c r="D27" s="65"/>
+      <c r="D27" s="79"/>
       <c r="E27" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="69"/>
+        <v>45</v>
+      </c>
+      <c r="F27" s="82"/>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
       <c r="I27" s="3"/>
@@ -2044,14 +2032,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="64"/>
-      <c r="B28" s="63"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="65"/>
+      <c r="D28" s="79"/>
       <c r="E28" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="69"/>
+        <v>65</v>
+      </c>
+      <c r="F28" s="82"/>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
       <c r="I28" s="3"/>
@@ -2074,14 +2062,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="27"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="79"/>
       <c r="E29" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="34"/>
+        <v>66</v>
+      </c>
+      <c r="F29" s="82"/>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
       <c r="I29" s="3"/>
@@ -2109,7 +2097,7 @@
       <c r="C30" s="22"/>
       <c r="D30" s="27"/>
       <c r="E30" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="39"/>
@@ -2139,7 +2127,7 @@
       <c r="C31" s="22"/>
       <c r="D31" s="27"/>
       <c r="E31" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="39"/>
@@ -2169,7 +2157,7 @@
       <c r="C32" s="22"/>
       <c r="D32" s="27"/>
       <c r="E32" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="39"/>
@@ -2199,7 +2187,7 @@
       <c r="C33" s="22"/>
       <c r="D33" s="27"/>
       <c r="E33" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="39"/>
@@ -2229,7 +2217,7 @@
       <c r="C34" s="22"/>
       <c r="D34" s="27"/>
       <c r="E34" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="39"/>
@@ -2253,13 +2241,13 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="19.8" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
       <c r="D35" s="27"/>
       <c r="E35" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="39"/>
@@ -2283,16 +2271,16 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="8" customFormat="1" ht="19.8" customHeight="1">
+    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.8" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
       <c r="D36" s="27"/>
       <c r="E36" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="34"/>
-      <c r="G36" s="40"/>
+      <c r="G36" s="39"/>
       <c r="H36" s="39"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -2319,7 +2307,7 @@
       <c r="C37" s="22"/>
       <c r="D37" s="27"/>
       <c r="E37" s="30" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="40"/>
@@ -2343,83 +2331,81 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="7" customFormat="1" ht="11.4" customHeight="1">
-      <c r="A38" s="17"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-    </row>
-    <row r="39" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A39" s="12">
+    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.8" customHeight="1">
+      <c r="A38" s="12"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="34"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+    </row>
+    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.4" customHeight="1">
+      <c r="A39" s="17"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+      <c r="A40" s="12">
         <v>3</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B40" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C40" s="22" t="s">
         <v>17</v>
-      </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-    </row>
-    <row r="40" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A40" s="12"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="22" t="s">
-        <v>18</v>
       </c>
       <c r="D40" s="28"/>
       <c r="E40" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="74"/>
+        <v>46</v>
+      </c>
+      <c r="F40" s="58" t="s">
+        <v>92</v>
+      </c>
       <c r="G40" s="12"/>
       <c r="H40" s="39"/>
       <c r="I40" s="3"/>
@@ -2445,13 +2431,13 @@
       <c r="A41" s="12"/>
       <c r="B41" s="20"/>
       <c r="C41" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" s="28"/>
       <c r="E41" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="F41" s="74"/>
+        <v>47</v>
+      </c>
+      <c r="F41" s="59"/>
       <c r="G41" s="12"/>
       <c r="H41" s="39"/>
       <c r="I41" s="3"/>
@@ -2476,12 +2462,14 @@
     <row r="42" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" s="20"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
+      <c r="C42" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="28"/>
       <c r="E42" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42" s="74"/>
+        <v>48</v>
+      </c>
+      <c r="F42" s="59"/>
       <c r="G42" s="12"/>
       <c r="H42" s="39"/>
       <c r="I42" s="3"/>
@@ -2506,14 +2494,12 @@
     <row r="43" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="20"/>
-      <c r="C43" s="22" t="s">
-        <v>20</v>
-      </c>
+      <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" s="75"/>
+        <v>110</v>
+      </c>
+      <c r="F43" s="59"/>
       <c r="G43" s="12"/>
       <c r="H43" s="39"/>
       <c r="I43" s="3"/>
@@ -2539,13 +2525,13 @@
       <c r="A44" s="12"/>
       <c r="B44" s="20"/>
       <c r="C44" s="22" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="D44" s="22"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="34" t="s">
-        <v>82</v>
-      </c>
+      <c r="E44" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="60"/>
       <c r="G44" s="12"/>
       <c r="H44" s="39"/>
       <c r="I44" s="3"/>
@@ -2567,143 +2553,147 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A45" s="17"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
-      <c r="U45" s="6"/>
-      <c r="V45" s="6"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-    </row>
-    <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A46" s="57">
+    <row r="45" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+      <c r="A45" s="12"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="G45" s="12"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+    </row>
+    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
+      <c r="A46" s="17"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
+      <c r="U46" s="6"/>
+      <c r="V46" s="6"/>
+      <c r="W46" s="6"/>
+      <c r="X46" s="6"/>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6"/>
+    </row>
+    <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A47" s="61">
         <v>4</v>
       </c>
-      <c r="B46" s="60" t="s">
+      <c r="B47" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C47" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="66"/>
-      <c r="E46" s="30" t="s">
+      <c r="D47" s="67"/>
+      <c r="E47" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="F46" s="54" t="s">
+      <c r="F47" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="G46" s="39" t="s">
+      <c r="G47" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="H46" s="39"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-    </row>
-    <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A47" s="58"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="25" t="s">
+      <c r="H47" s="39"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+    </row>
+    <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A48" s="62"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="76"/>
-      <c r="E47" s="32" t="s">
+      <c r="D48" s="68"/>
+      <c r="E48" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="74"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
-      <c r="X47" s="9"/>
-      <c r="Y47" s="9"/>
-      <c r="Z47" s="9"/>
-    </row>
-    <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A48" s="58"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="22" t="s">
+      <c r="F48" s="59"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="9"/>
+      <c r="Y48" s="9"/>
+      <c r="Z48" s="9"/>
+    </row>
+    <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A49" s="62"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="76"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-    </row>
-    <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="58"/>
-      <c r="B49" s="61"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="74"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="59"/>
       <c r="G49" s="39"/>
       <c r="H49" s="39"/>
       <c r="I49" s="3"/>
@@ -2725,13 +2715,13 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="59"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="75"/>
+    <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A50" s="62"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="59"/>
       <c r="G50" s="39"/>
       <c r="H50" s="39"/>
       <c r="I50" s="3"/>
@@ -2753,82 +2743,80 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A51" s="17"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="6"/>
-      <c r="U51" s="6"/>
-      <c r="V51" s="6"/>
-      <c r="W51" s="6"/>
-      <c r="X51" s="6"/>
-      <c r="Y51" s="6"/>
-      <c r="Z51" s="6"/>
-    </row>
-    <row r="52" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A52" s="64">
+    <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A51" s="63"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+    </row>
+    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
+      <c r="A52" s="17"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="6"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="6"/>
+      <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+    </row>
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A53" s="78">
         <v>5</v>
       </c>
-      <c r="B52" s="63" t="s">
+      <c r="B53" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C53" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="30" t="s">
+      <c r="D53" s="28"/>
+      <c r="E53" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F52" s="54" t="s">
+      <c r="F53" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="G52" s="12"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
-      <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
-      <c r="Z52" s="3"/>
-    </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A53" s="64"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="42"/>
+      <c r="G53" s="12"/>
       <c r="H53" s="39"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -2850,15 +2838,15 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="64"/>
-      <c r="B54" s="63"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="77"/>
       <c r="C54" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="12"/>
+      <c r="F54" s="83"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="39"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -2879,79 +2867,80 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="A55" s="17"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-      <c r="S55" s="6"/>
-      <c r="T55" s="6"/>
-      <c r="U55" s="6"/>
-      <c r="V55" s="6"/>
-      <c r="W55" s="6"/>
-      <c r="X55" s="6"/>
-      <c r="Y55" s="6"/>
-      <c r="Z55" s="6"/>
-    </row>
-    <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="64">
+    <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A55" s="78"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="28"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="84"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
+      <c r="X55" s="3"/>
+      <c r="Y55" s="3"/>
+      <c r="Z55" s="3"/>
+    </row>
+    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
+      <c r="A56" s="17"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="6"/>
+      <c r="Q56" s="6"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+      <c r="U56" s="6"/>
+      <c r="V56" s="6"/>
+      <c r="W56" s="6"/>
+      <c r="X56" s="6"/>
+      <c r="Y56" s="6"/>
+      <c r="Z56" s="6"/>
+    </row>
+    <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A57" s="78">
         <v>6</v>
       </c>
-      <c r="B56" s="63" t="s">
+      <c r="B57" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="65"/>
-      <c r="E56" s="30" t="s">
+      <c r="C57" s="24"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F56" s="54" t="s">
+      <c r="F57" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
-      <c r="R56" s="3"/>
-      <c r="S56" s="3"/>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
-      <c r="V56" s="3"/>
-      <c r="W56" s="3"/>
-      <c r="X56" s="3"/>
-      <c r="Y56" s="3"/>
-      <c r="Z56" s="3"/>
-    </row>
-    <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A57" s="64"/>
-      <c r="B57" s="63"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="F57" s="55"/>
-      <c r="G57" s="42"/>
+      <c r="G57" s="12"/>
       <c r="H57" s="39"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
@@ -2972,17 +2961,14 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A58" s="64"/>
-      <c r="B58" s="63"/>
-      <c r="C58" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" s="66"/>
+    <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A58" s="78"/>
+      <c r="B58" s="77"/>
+      <c r="D58" s="79"/>
       <c r="E58" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F58" s="56"/>
+        <v>77</v>
+      </c>
+      <c r="F58" s="83"/>
       <c r="G58" s="42"/>
       <c r="H58" s="39"/>
       <c r="I58" s="3"/>
@@ -3004,15 +2990,17 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A59" s="50"/>
-      <c r="B59" s="49"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="F59" s="52"/>
+    <row r="59" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A59" s="78"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="67"/>
+      <c r="E59" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="84"/>
       <c r="G59" s="42"/>
       <c r="H59" s="39"/>
       <c r="I59" s="3"/>
@@ -3040,7 +3028,7 @@
       <c r="C60" s="53"/>
       <c r="D60" s="29"/>
       <c r="E60" s="51" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F60" s="52"/>
       <c r="G60" s="42"/>
@@ -3064,149 +3052,147 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="7" customFormat="1" ht="22.8" customHeight="1">
-      <c r="A61" s="17"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
-      <c r="P61" s="6"/>
-      <c r="Q61" s="6"/>
-      <c r="R61" s="6"/>
-      <c r="S61" s="6"/>
-      <c r="T61" s="6"/>
-      <c r="U61" s="6"/>
-      <c r="V61" s="6"/>
-      <c r="W61" s="6"/>
-      <c r="X61" s="6"/>
-      <c r="Y61" s="6"/>
-      <c r="Z61" s="6"/>
-    </row>
-    <row r="62" spans="1:26" s="4" customFormat="1" ht="67.8" customHeight="1">
-      <c r="A62" s="12">
+    <row r="61" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
+      <c r="A61" s="50"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F61" s="52"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="V61" s="3"/>
+      <c r="W61" s="3"/>
+      <c r="X61" s="3"/>
+      <c r="Y61" s="3"/>
+      <c r="Z61" s="3"/>
+    </row>
+    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.8" customHeight="1">
+      <c r="A62" s="17"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="6"/>
+      <c r="T62" s="6"/>
+      <c r="U62" s="6"/>
+      <c r="V62" s="6"/>
+      <c r="W62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+      <c r="Z62" s="6"/>
+    </row>
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.8" customHeight="1">
+      <c r="A63" s="12">
         <v>7</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B63" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C63" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D62" s="27"/>
-      <c r="E62" s="33" t="s">
+      <c r="D63" s="27"/>
+      <c r="E63" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="F62" s="36" t="s">
+      <c r="F63" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="G62" s="42"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-      <c r="Q62" s="3"/>
-      <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
-      <c r="W62" s="3"/>
-      <c r="X62" s="3"/>
-      <c r="Y62" s="3"/>
-      <c r="Z62" s="3"/>
-    </row>
-    <row r="63" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
-      <c r="A63" s="17"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="6"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
-      <c r="L63" s="6"/>
-      <c r="M63" s="6"/>
-      <c r="N63" s="6"/>
-      <c r="O63" s="6"/>
-      <c r="P63" s="6"/>
-      <c r="Q63" s="6"/>
-      <c r="R63" s="6"/>
-      <c r="S63" s="6"/>
-      <c r="T63" s="6"/>
-      <c r="U63" s="6"/>
-      <c r="V63" s="6"/>
-      <c r="W63" s="6"/>
-      <c r="X63" s="6"/>
-      <c r="Y63" s="6"/>
-      <c r="Z63" s="6"/>
-    </row>
-    <row r="64" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A64" s="57">
+      <c r="G63" s="42"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="3"/>
+    </row>
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
+      <c r="A64" s="17"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+      <c r="V64" s="6"/>
+      <c r="W64" s="6"/>
+      <c r="X64" s="6"/>
+      <c r="Y64" s="6"/>
+      <c r="Z64" s="6"/>
+    </row>
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A65" s="61">
         <v>8</v>
       </c>
-      <c r="B64" s="60" t="s">
+      <c r="B65" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C65" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="D64" s="27"/>
-      <c r="E64" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="F64" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="G64" s="42"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-      <c r="O64" s="3"/>
-      <c r="P64" s="3"/>
-      <c r="Q64" s="3"/>
-      <c r="R64" s="3"/>
-      <c r="S64" s="3"/>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
-      <c r="V64" s="3"/>
-      <c r="W64" s="3"/>
-      <c r="X64" s="3"/>
-      <c r="Y64" s="3"/>
-      <c r="Z64" s="3"/>
-    </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="58"/>
-      <c r="B65" s="61"/>
-      <c r="C65" s="22" t="s">
-        <v>86</v>
       </c>
       <c r="D65" s="27"/>
       <c r="E65" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F65" s="55"/>
+        <v>49</v>
+      </c>
+      <c r="F65" s="58" t="s">
+        <v>98</v>
+      </c>
       <c r="G65" s="42"/>
       <c r="H65" s="39"/>
       <c r="I65" s="3"/>
@@ -3229,17 +3215,17 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="58"/>
-      <c r="B66" s="61"/>
+      <c r="A66" s="62"/>
+      <c r="B66" s="65"/>
       <c r="C66" s="22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D66" s="27"/>
       <c r="E66" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F66" s="55"/>
-      <c r="G66" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="F66" s="83"/>
+      <c r="G66" s="42"/>
       <c r="H66" s="39"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
@@ -3261,12 +3247,16 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="59"/>
-      <c r="B67" s="62"/>
-      <c r="C67" s="22"/>
+      <c r="A67" s="62"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="22" t="s">
+        <v>85</v>
+      </c>
       <c r="D67" s="27"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="56"/>
+      <c r="E67" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F67" s="83"/>
       <c r="G67" s="12"/>
       <c r="H67" s="39"/>
       <c r="I67" s="3"/>
@@ -3288,106 +3278,134 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
-      <c r="A68" s="17"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
-      <c r="N68" s="6"/>
-      <c r="O68" s="6"/>
-      <c r="P68" s="6"/>
-      <c r="Q68" s="6"/>
-      <c r="R68" s="6"/>
-      <c r="S68" s="6"/>
-      <c r="T68" s="6"/>
-      <c r="U68" s="6"/>
-      <c r="V68" s="6"/>
-      <c r="W68" s="6"/>
-      <c r="X68" s="6"/>
-      <c r="Y68" s="6"/>
-      <c r="Z68" s="6"/>
-    </row>
-    <row r="69" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A69" s="12">
+    <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A68" s="63"/>
+      <c r="B68" s="66"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="84"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3"/>
+    </row>
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+      <c r="A69" s="17"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+      <c r="U69" s="6"/>
+      <c r="V69" s="6"/>
+      <c r="W69" s="6"/>
+      <c r="X69" s="6"/>
+      <c r="Y69" s="6"/>
+      <c r="Z69" s="6"/>
+    </row>
+    <row r="70" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A70" s="12">
         <v>9</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B70" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="31" t="s">
+      <c r="C70" s="22"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="F69" s="36" t="s">
+      <c r="F70" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="G69" s="12"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
-      <c r="O69" s="3"/>
-      <c r="P69" s="3"/>
-      <c r="Q69" s="3"/>
-      <c r="R69" s="3"/>
-      <c r="S69" s="3"/>
-      <c r="T69" s="3"/>
-      <c r="U69" s="3"/>
-      <c r="V69" s="3"/>
-      <c r="W69" s="3"/>
-      <c r="X69" s="3"/>
-      <c r="Y69" s="3"/>
-      <c r="Z69" s="3"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
+      <c r="X70" s="3"/>
+      <c r="Y70" s="3"/>
+      <c r="Z70" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="D11:D29"/>
+    <mergeCell ref="F11:F29"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="F39:F43"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="F47:F51"/>
+    <mergeCell ref="F40:F44"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="E49:E51"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B28"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A10:A28"/>
-    <mergeCell ref="D10:D28"/>
-    <mergeCell ref="F10:F28"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B29"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -3398,7 +3416,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
+  <conditionalFormatting sqref="C7:E7">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -3410,7 +3428,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" display="2.0.3"/>
+    <hyperlink ref="E8" r:id="rId1" display="2.0.3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
update the RTM and SDD -Aya
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\ProjectManagement\project\Learning-hub\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AyaMohamed\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7764"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
   <si>
     <t>Project Name:</t>
   </si>
@@ -409,6 +409,21 @@
   </si>
   <si>
     <t>Lhub_SRS_2.4.3.13</t>
+  </si>
+  <si>
+    <t>login_user(string username , string password)</t>
+  </si>
+  <si>
+    <t>signup_user(string username, string password, string fname, string lname, string email)</t>
+  </si>
+  <si>
+    <t>followCategory(username, categoryName)</t>
+  </si>
+  <si>
+    <t>reviewArticle(option , author, title)</t>
+  </si>
+  <si>
+    <t>resetPassword(email,password)</t>
   </si>
 </sst>
 </file>
@@ -686,7 +701,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -785,9 +800,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -833,6 +845,63 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,34 +914,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -896,35 +941,11 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1253,42 +1274,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="23.21875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="48.21875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="54.21875" style="21" customWidth="1"/>
-    <col min="7" max="7" width="69.5546875" style="18" customWidth="1"/>
-    <col min="8" max="8" width="44.5546875" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="5"/>
+    <col min="1" max="1" width="23.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="54.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="78.42578125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.8" customHeight="1">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="45"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="75"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="13" t="s">
         <v>51</v>
       </c>
@@ -1306,13 +1327,13 @@
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="85"/>
       <c r="D3" s="14">
         <v>1</v>
       </c>
@@ -1322,21 +1343,21 @@
       <c r="F3" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="46" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="76">
+      <c r="B4" s="86">
         <v>43470</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="86"/>
       <c r="D4" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -1346,44 +1367,44 @@
       <c r="F4" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="46" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="44"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="14">
         <v>1.2</v>
       </c>
       <c r="E5" s="15">
         <v>43601</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A6" s="44"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-    </row>
-    <row r="7" spans="1:26" s="46" customFormat="1" ht="93" customHeight="1">
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+    </row>
+    <row r="7" spans="1:26" s="45" customFormat="1" ht="93" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1409,23 +1430,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.799999999999997" customHeight="1">
-      <c r="A8" s="78">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
+      <c r="A8" s="66">
         <v>1</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="65" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="80"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="80"/>
+      <c r="H8" s="69"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1446,18 +1467,18 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="77"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="79"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="80"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="80"/>
+      <c r="H9" s="69"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1477,7 +1498,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.8" customHeight="1">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.9" customHeight="1">
       <c r="A10" s="17"/>
       <c r="B10" s="19"/>
       <c r="C10" s="23"/>
@@ -1505,25 +1526,27 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="18" customHeight="1">
-      <c r="A11" s="78">
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A11" s="66">
         <v>2</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="65" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="79"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="78"/>
+      <c r="G11" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="66"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1543,19 +1566,18 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A12" s="78"/>
-      <c r="B12" s="77"/>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
+      <c r="A12" s="66"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="79"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="82"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="78"/>
+      <c r="F12" s="71"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1576,18 +1598,18 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="78"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="79"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="82"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1608,18 +1630,18 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="78"/>
-      <c r="B14" s="77"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="79"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="82"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1640,18 +1662,18 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="78"/>
-      <c r="B15" s="77"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="79"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1672,16 +1694,16 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="78"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="79"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="82"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1702,16 +1724,16 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="78"/>
-      <c r="B17" s="77"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="79"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="82"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1732,16 +1754,16 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="78"/>
-      <c r="B18" s="77"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="79"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="82"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1762,16 +1784,16 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="78"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="24"/>
-      <c r="D19" s="79"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="82"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1792,16 +1814,16 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="78"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="24"/>
-      <c r="D20" s="79"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="82"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1822,16 +1844,18 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="78"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="24"/>
-      <c r="D21" s="79"/>
+      <c r="D21" s="67"/>
       <c r="E21" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="82"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="38"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1852,16 +1876,16 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="78"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="24"/>
-      <c r="D22" s="79"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="82"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1882,16 +1906,16 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="78"/>
-      <c r="B23" s="77"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="79"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="82"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1912,16 +1936,16 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="78"/>
-      <c r="B24" s="77"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="79"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="82"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1941,17 +1965,19 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="78"/>
-      <c r="B25" s="77"/>
+    <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
+      <c r="A25" s="66"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="79"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="82"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" s="38"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1972,16 +1998,16 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="78"/>
-      <c r="B26" s="77"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="79"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="82"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2002,16 +2028,16 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="78"/>
-      <c r="B27" s="77"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="24"/>
-      <c r="D27" s="79"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="82"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2032,16 +2058,16 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="78"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="79"/>
+      <c r="D28" s="67"/>
       <c r="E28" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="82"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2062,16 +2088,16 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="78"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="24"/>
-      <c r="D29" s="79"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="82"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2100,8 +2126,8 @@
         <v>67</v>
       </c>
       <c r="F30" s="34"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2130,8 +2156,8 @@
         <v>68</v>
       </c>
       <c r="F31" s="34"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2160,8 +2186,8 @@
         <v>69</v>
       </c>
       <c r="F32" s="34"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2190,8 +2216,8 @@
         <v>70</v>
       </c>
       <c r="F33" s="34"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2220,8 +2246,8 @@
         <v>71</v>
       </c>
       <c r="F34" s="34"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2250,8 +2276,8 @@
         <v>72</v>
       </c>
       <c r="F35" s="34"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2271,7 +2297,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.8" customHeight="1">
+    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
@@ -2280,8 +2306,8 @@
         <v>73</v>
       </c>
       <c r="F36" s="34"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2301,7 +2327,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.8" customHeight="1">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A37" s="12"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
@@ -2310,8 +2336,8 @@
         <v>74</v>
       </c>
       <c r="F37" s="34"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="38"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2331,7 +2357,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.8" customHeight="1">
+    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A38" s="12"/>
       <c r="B38" s="20"/>
       <c r="C38" s="22"/>
@@ -2340,8 +2366,8 @@
         <v>102</v>
       </c>
       <c r="F38" s="34"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="38"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2361,15 +2387,15 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.4" customHeight="1">
+    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="19"/>
       <c r="C39" s="23"/>
       <c r="D39" s="26"/>
       <c r="E39" s="19"/>
       <c r="F39" s="35"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="43"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="42"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -2403,11 +2429,11 @@
       <c r="E40" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="58" t="s">
+      <c r="F40" s="56" t="s">
         <v>92</v>
       </c>
       <c r="G40" s="12"/>
-      <c r="H40" s="39"/>
+      <c r="H40" s="38"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2437,9 +2463,9 @@
       <c r="E41" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="59"/>
+      <c r="F41" s="76"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="39"/>
+      <c r="H41" s="38"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2469,9 +2495,9 @@
       <c r="E42" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="59"/>
+      <c r="F42" s="76"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="39"/>
+      <c r="H42" s="38"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2499,9 +2525,9 @@
       <c r="E43" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="59"/>
+      <c r="F43" s="76"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="39"/>
+      <c r="H43" s="38"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2531,9 +2557,9 @@
       <c r="E44" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="60"/>
+      <c r="F44" s="77"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="39"/>
+      <c r="H44" s="38"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2565,7 +2591,7 @@
         <v>82</v>
       </c>
       <c r="G45" s="12"/>
-      <c r="H45" s="39"/>
+      <c r="H45" s="38"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2593,7 +2619,7 @@
       <c r="E46" s="19"/>
       <c r="F46" s="35"/>
       <c r="G46" s="17"/>
-      <c r="H46" s="43"/>
+      <c r="H46" s="42"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2614,26 +2640,26 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="61">
+      <c r="A47" s="59">
         <v>4</v>
       </c>
-      <c r="B47" s="64" t="s">
+      <c r="B47" s="62" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="67"/>
+      <c r="D47" s="68"/>
       <c r="E47" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="58" t="s">
+      <c r="F47" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="G47" s="39" t="s">
+      <c r="G47" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="H47" s="39"/>
+      <c r="H47" s="38"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -2654,18 +2680,18 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="62"/>
-      <c r="B48" s="65"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="63"/>
       <c r="C48" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="68"/>
+      <c r="D48" s="78"/>
       <c r="E48" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="59"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
+      <c r="F48" s="76"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2686,16 +2712,16 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="62"/>
-      <c r="B49" s="65"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="63"/>
       <c r="C49" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="68"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2716,14 +2742,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="62"/>
-      <c r="B50" s="65"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
+      <c r="A50" s="60"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="78"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2744,14 +2770,14 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="63"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2779,7 +2805,7 @@
       <c r="E52" s="19"/>
       <c r="F52" s="35"/>
       <c r="G52" s="17"/>
-      <c r="H52" s="43"/>
+      <c r="H52" s="42"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -2800,10 +2826,10 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A53" s="78">
+      <c r="A53" s="66">
         <v>5</v>
       </c>
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="65" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="22" t="s">
@@ -2813,11 +2839,11 @@
       <c r="E53" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="58" t="s">
+      <c r="F53" s="56" t="s">
         <v>94</v>
       </c>
       <c r="G53" s="12"/>
-      <c r="H53" s="39"/>
+      <c r="H53" s="38"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2838,16 +2864,16 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="78"/>
-      <c r="B54" s="77"/>
+      <c r="A54" s="66"/>
+      <c r="B54" s="65"/>
       <c r="C54" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="39"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="38"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2868,16 +2894,16 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="78"/>
-      <c r="B55" s="77"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="65"/>
       <c r="C55" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="28"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="84"/>
+      <c r="F55" s="58"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="39"/>
+      <c r="H55" s="38"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2905,7 +2931,7 @@
       <c r="E56" s="19"/>
       <c r="F56" s="35"/>
       <c r="G56" s="17"/>
-      <c r="H56" s="43"/>
+      <c r="H56" s="42"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -2926,22 +2952,22 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="78">
+      <c r="A57" s="66">
         <v>6</v>
       </c>
-      <c r="B57" s="77" t="s">
+      <c r="B57" s="65" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="24"/>
-      <c r="D57" s="79"/>
+      <c r="D57" s="67"/>
       <c r="E57" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F57" s="58" t="s">
+      <c r="F57" s="56" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="12"/>
-      <c r="H57" s="39"/>
+      <c r="H57" s="38"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2962,15 +2988,15 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="78"/>
-      <c r="B58" s="77"/>
-      <c r="D58" s="79"/>
+      <c r="A58" s="66"/>
+      <c r="B58" s="65"/>
+      <c r="D58" s="67"/>
       <c r="E58" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="83"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="39"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="38"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -2990,19 +3016,19 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A59" s="78"/>
-      <c r="B59" s="77"/>
+    <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
+      <c r="A59" s="66"/>
+      <c r="B59" s="65"/>
       <c r="C59" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="67"/>
+      <c r="D59" s="68"/>
       <c r="E59" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="84"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="39"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="38"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3023,16 +3049,16 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A60" s="50"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="53"/>
+      <c r="A60" s="49"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="52"/>
       <c r="D60" s="29"/>
-      <c r="E60" s="51" t="s">
+      <c r="E60" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="52"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="39"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="38"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3053,16 +3079,16 @@
       <c r="Z60" s="3"/>
     </row>
     <row r="61" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A61" s="50"/>
-      <c r="B61" s="49"/>
-      <c r="C61" s="53"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="52"/>
       <c r="D61" s="29"/>
-      <c r="E61" s="51" t="s">
+      <c r="E61" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F61" s="52"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="39"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="38"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3082,7 +3108,7 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.8" customHeight="1">
+    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.9" customHeight="1">
       <c r="A62" s="17"/>
       <c r="B62" s="19"/>
       <c r="C62" s="23"/>
@@ -3090,7 +3116,7 @@
       <c r="E62" s="19"/>
       <c r="F62" s="35"/>
       <c r="G62" s="17"/>
-      <c r="H62" s="43"/>
+      <c r="H62" s="42"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -3110,7 +3136,7 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.8" customHeight="1">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1">
       <c r="A63" s="12">
         <v>7</v>
       </c>
@@ -3127,8 +3153,10 @@
       <c r="F63" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="G63" s="42"/>
-      <c r="H63" s="39"/>
+      <c r="G63" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="H63" s="38"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3148,7 +3176,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1">
       <c r="A64" s="17"/>
       <c r="B64" s="19"/>
       <c r="C64" s="23"/>
@@ -3156,7 +3184,7 @@
       <c r="E64" s="19"/>
       <c r="F64" s="35"/>
       <c r="G64" s="17"/>
-      <c r="H64" s="43"/>
+      <c r="H64" s="42"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3177,10 +3205,10 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="61">
+      <c r="A65" s="59">
         <v>8</v>
       </c>
-      <c r="B65" s="64" t="s">
+      <c r="B65" s="62" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="22" t="s">
@@ -3190,11 +3218,13 @@
       <c r="E65" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="58" t="s">
+      <c r="F65" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="G65" s="42"/>
-      <c r="H65" s="39"/>
+      <c r="G65" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H65" s="38"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3215,8 +3245,8 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="62"/>
-      <c r="B66" s="65"/>
+      <c r="A66" s="60"/>
+      <c r="B66" s="63"/>
       <c r="C66" s="22" t="s">
         <v>86</v>
       </c>
@@ -3224,9 +3254,9 @@
       <c r="E66" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F66" s="83"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="39"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="38"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -3247,8 +3277,8 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="62"/>
-      <c r="B67" s="65"/>
+      <c r="A67" s="60"/>
+      <c r="B67" s="63"/>
       <c r="C67" s="22" t="s">
         <v>85</v>
       </c>
@@ -3256,9 +3286,9 @@
       <c r="E67" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="83"/>
+      <c r="F67" s="57"/>
       <c r="G67" s="12"/>
-      <c r="H67" s="39"/>
+      <c r="H67" s="38"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -3279,14 +3309,14 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="63"/>
-      <c r="B68" s="66"/>
+      <c r="A68" s="61"/>
+      <c r="B68" s="64"/>
       <c r="C68" s="22"/>
       <c r="D68" s="27"/>
       <c r="E68" s="21"/>
-      <c r="F68" s="84"/>
+      <c r="F68" s="58"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="39"/>
+      <c r="H68" s="38"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -3306,7 +3336,7 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.149999999999999" customHeight="1">
       <c r="A69" s="17"/>
       <c r="B69" s="19"/>
       <c r="C69" s="23"/>
@@ -3314,7 +3344,7 @@
       <c r="E69" s="19"/>
       <c r="F69" s="35"/>
       <c r="G69" s="17"/>
-      <c r="H69" s="43"/>
+      <c r="H69" s="42"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -3350,7 +3380,7 @@
         <v>97</v>
       </c>
       <c r="G70" s="12"/>
-      <c r="H70" s="39"/>
+      <c r="H70" s="38"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3372,22 +3402,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="D11:D29"/>
-    <mergeCell ref="F11:F29"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3404,6 +3418,22 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="D11:D29"/>
+    <mergeCell ref="F11:F29"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
update the SRS IDs column according to SRS document as SRS login module was updated
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AyaMohamed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7152"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="121">
   <si>
     <t>Project Name:</t>
   </si>
@@ -425,6 +425,9 @@
   <si>
     <t>resetPassword(email,password)</t>
   </si>
+  <si>
+    <t>update the SRS IDs column according to SRS document as SRS login module was updated</t>
+  </si>
 </sst>
 </file>
 
@@ -433,11 +436,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -449,7 +452,7 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -484,12 +487,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -549,7 +546,7 @@
       <b/>
       <sz val="24"/>
       <color theme="0"/>
-      <name val="Calibri Light"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -701,7 +698,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -729,223 +726,226 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1050,22 +1050,22 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Arial">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Arial" panose="020B0604020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Hang" typeface="굴림"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
         <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Cans" typeface="Euphemia"/>
@@ -1082,21 +1082,21 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Arial" panose="020B0604020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Hang" typeface="굴림"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -1274,137 +1274,145 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="54.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="78.42578125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.28515625" style="5"/>
+    <col min="1" max="1" width="23.296875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.3984375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="48.296875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="28.796875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="35.59765625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="54.296875" style="20" customWidth="1"/>
+    <col min="7" max="7" width="78.3984375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="44.5" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="9.296875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="72" t="s">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.95" customHeight="1">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="44"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="89" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="14">
+      <c r="C3" s="78"/>
+      <c r="D3" s="13">
         <v>1</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>43588</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="45" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="86">
+      <c r="B4" s="79">
         <v>43470</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="14">
+      <c r="C4" s="79"/>
+      <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>43592</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="45" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="14">
+      <c r="A5" s="42"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="13">
         <v>1.2</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>43601</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-    </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="93" customHeight="1">
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.2" customHeight="1">
+      <c r="A6" s="42"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="E6" s="14">
+        <v>43608</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1430,23 +1438,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
-      <c r="A8" s="66">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
+      <c r="A8" s="81">
         <v>1</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="82"/>
+      <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="69"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="83"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1467,18 +1475,18 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="66"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="22" t="s">
+      <c r="A9" s="81"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="67"/>
-      <c r="E9" s="30" t="s">
+      <c r="D9" s="82"/>
+      <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="69"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="83"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1498,15 +1506,15 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1527,26 +1535,26 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="66">
+      <c r="A11" s="81">
         <v>2</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="30" t="s">
+      <c r="D11" s="82"/>
+      <c r="E11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="G11" s="87" t="s">
+      <c r="G11" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="66"/>
+      <c r="H11" s="81"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1567,17 +1575,17 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="66"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="22" t="s">
+      <c r="A12" s="81"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="82"/>
+      <c r="E12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="71"/>
-      <c r="H12" s="66"/>
+      <c r="F12" s="85"/>
+      <c r="H12" s="81"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1598,18 +1606,18 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="66"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="22" t="s">
+      <c r="A13" s="81"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="82"/>
+      <c r="E13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1630,18 +1638,18 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="66"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="22" t="s">
+      <c r="A14" s="81"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="30" t="s">
+      <c r="D14" s="82"/>
+      <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="71"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1662,18 +1670,18 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="66"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="22" t="s">
+      <c r="A15" s="81"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="30" t="s">
+      <c r="D15" s="82"/>
+      <c r="E15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="71"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1694,16 +1702,16 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="66"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="30" t="s">
+      <c r="A16" s="81"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1724,16 +1732,16 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="66"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="30" t="s">
+      <c r="A17" s="81"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="71"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1754,16 +1762,16 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="66"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="30" t="s">
+      <c r="A18" s="81"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="71"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1784,16 +1792,16 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="66"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="30" t="s">
+      <c r="A19" s="81"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="71"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1814,16 +1822,16 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="66"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="30" t="s">
+      <c r="A20" s="81"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="71"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1844,18 +1852,18 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="66"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="30" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="71"/>
-      <c r="G21" s="53" t="s">
+      <c r="F21" s="85"/>
+      <c r="G21" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1876,16 +1884,16 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="66"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="30" t="s">
+      <c r="A22" s="81"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="71"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1906,16 +1914,16 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="66"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="30" t="s">
+      <c r="A23" s="81"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="71"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1936,16 +1944,16 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="66"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="30" t="s">
+      <c r="A24" s="81"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="71"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1966,18 +1974,18 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="66"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="30" t="s">
+      <c r="A25" s="81"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="71"/>
-      <c r="G25" s="88" t="s">
+      <c r="F25" s="85"/>
+      <c r="G25" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="H25" s="38"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1998,16 +2006,16 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="66"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="30" t="s">
+      <c r="A26" s="81"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="71"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2028,16 +2036,16 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="66"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="30" t="s">
+      <c r="A27" s="81"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="71"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2058,16 +2066,16 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="66"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="30" t="s">
+      <c r="A28" s="81"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2088,16 +2096,16 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="66"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="30" t="s">
+      <c r="A29" s="81"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="71"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2119,15 +2127,15 @@
     </row>
     <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A30" s="12"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="30" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2149,15 +2157,15 @@
     </row>
     <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A31" s="12"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="30" t="s">
+      <c r="B31" s="19"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="34"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2179,15 +2187,15 @@
     </row>
     <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A32" s="12"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="30" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2209,15 +2217,15 @@
     </row>
     <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A33" s="12"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="30" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2239,15 +2247,15 @@
     </row>
     <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A34" s="12"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="30" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2269,15 +2277,15 @@
     </row>
     <row r="35" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A35" s="12"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="30" t="s">
+      <c r="B35" s="19"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2297,17 +2305,17 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A36" s="12"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="30" t="s">
+      <c r="B36" s="19"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2327,17 +2335,17 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
       <c r="A37" s="12"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="30" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="34"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="38"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="37"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2357,17 +2365,17 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
       <c r="A38" s="12"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="30" t="s">
+      <c r="B38" s="19"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F38" s="34"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="38"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="37"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2387,15 +2395,15 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1">
-      <c r="A39" s="17"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="42"/>
+    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.4" customHeight="1">
+      <c r="A39" s="16"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="41"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -2419,21 +2427,21 @@
       <c r="A40" s="12">
         <v>3</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="31" t="s">
+      <c r="D40" s="27"/>
+      <c r="E40" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="56" t="s">
+      <c r="F40" s="61" t="s">
         <v>92</v>
       </c>
       <c r="G40" s="12"/>
-      <c r="H40" s="38"/>
+      <c r="H40" s="37"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2455,17 +2463,17 @@
     </row>
     <row r="41" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A41" s="12"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="22" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="31" t="s">
+      <c r="D41" s="27"/>
+      <c r="E41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="76"/>
+      <c r="F41" s="62"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="38"/>
+      <c r="H41" s="37"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2487,17 +2495,17 @@
     </row>
     <row r="42" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A42" s="12"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="22" t="s">
+      <c r="B42" s="19"/>
+      <c r="C42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="31" t="s">
+      <c r="D42" s="27"/>
+      <c r="E42" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="76"/>
+      <c r="F42" s="62"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="38"/>
+      <c r="H42" s="37"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2519,15 +2527,15 @@
     </row>
     <row r="43" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A43" s="12"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="31" t="s">
+      <c r="B43" s="19"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="76"/>
+      <c r="F43" s="62"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="38"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2549,17 +2557,17 @@
     </row>
     <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A44" s="12"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="22" t="s">
+      <c r="B44" s="19"/>
+      <c r="C44" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="31" t="s">
+      <c r="D44" s="21"/>
+      <c r="E44" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="77"/>
+      <c r="F44" s="63"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="38"/>
+      <c r="H44" s="37"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2581,17 +2589,17 @@
     </row>
     <row r="45" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A45" s="12"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="22" t="s">
+      <c r="B45" s="19"/>
+      <c r="C45" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="34" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="33" t="s">
         <v>82</v>
       </c>
       <c r="G45" s="12"/>
-      <c r="H45" s="38"/>
+      <c r="H45" s="37"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2612,14 +2620,14 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A46" s="17"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="42"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="41"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2640,26 +2648,26 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="59">
+      <c r="A47" s="64">
         <v>4</v>
       </c>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="68"/>
-      <c r="E47" s="30" t="s">
+      <c r="D47" s="70"/>
+      <c r="E47" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="56" t="s">
+      <c r="F47" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="G47" s="38" t="s">
+      <c r="G47" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="H47" s="38"/>
+      <c r="H47" s="37"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -2680,18 +2688,18 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="60"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="25" t="s">
+      <c r="A48" s="65"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="78"/>
-      <c r="E48" s="32" t="s">
+      <c r="D48" s="71"/>
+      <c r="E48" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="76"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2712,16 +2720,16 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="22" t="s">
+      <c r="A49" s="65"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="78"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2742,14 +2750,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="60"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
+      <c r="A50" s="65"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2770,14 +2778,14 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="61"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="69"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2798,14 +2806,14 @@
       <c r="Z51" s="3"/>
     </row>
     <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A52" s="17"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="42"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="41"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -2826,24 +2834,24 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A53" s="66">
+      <c r="A53" s="81">
         <v>5</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="30" t="s">
+      <c r="D53" s="27"/>
+      <c r="E53" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="56" t="s">
+      <c r="F53" s="61" t="s">
         <v>94</v>
       </c>
       <c r="G53" s="12"/>
-      <c r="H53" s="38"/>
+      <c r="H53" s="37"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2864,16 +2872,16 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="66"/>
-      <c r="B54" s="65"/>
-      <c r="C54" s="22" t="s">
+      <c r="A54" s="81"/>
+      <c r="B54" s="80"/>
+      <c r="C54" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="38"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="37"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2894,16 +2902,16 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="66"/>
-      <c r="B55" s="65"/>
-      <c r="C55" s="22" t="s">
+      <c r="A55" s="81"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="28"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="58"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="87"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="38"/>
+      <c r="H55" s="37"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2924,14 +2932,14 @@
       <c r="Z55" s="3"/>
     </row>
     <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="A56" s="17"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="42"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="41"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -2952,22 +2960,22 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="66">
+      <c r="A57" s="81">
         <v>6</v>
       </c>
-      <c r="B57" s="65" t="s">
+      <c r="B57" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="67"/>
-      <c r="E57" s="30" t="s">
+      <c r="C57" s="23"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F57" s="56" t="s">
+      <c r="F57" s="61" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="12"/>
-      <c r="H57" s="38"/>
+      <c r="H57" s="37"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2988,15 +2996,15 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="66"/>
-      <c r="B58" s="65"/>
-      <c r="D58" s="67"/>
-      <c r="E58" s="30" t="s">
+      <c r="A58" s="81"/>
+      <c r="B58" s="80"/>
+      <c r="D58" s="82"/>
+      <c r="E58" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="57"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="38"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="37"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3017,18 +3025,18 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="66"/>
-      <c r="B59" s="65"/>
-      <c r="C59" s="22" t="s">
+      <c r="A59" s="81"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="68"/>
-      <c r="E59" s="30" t="s">
+      <c r="D59" s="70"/>
+      <c r="E59" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="58"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="38"/>
+      <c r="F59" s="87"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="37"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3049,16 +3057,16 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A60" s="49"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="50" t="s">
+      <c r="A60" s="48"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="51"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="38"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="37"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3079,16 +3087,16 @@
       <c r="Z60" s="3"/>
     </row>
     <row r="61" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A61" s="49"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="50" t="s">
+      <c r="A61" s="48"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F61" s="51"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="38"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="37"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3108,15 +3116,15 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.9" customHeight="1">
-      <c r="A62" s="17"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="42"/>
+    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.95" customHeight="1">
+      <c r="A62" s="16"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="41"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -3136,27 +3144,27 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.95" customHeight="1">
       <c r="A63" s="12">
         <v>7</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="27"/>
-      <c r="E63" s="33" t="s">
+      <c r="D63" s="26"/>
+      <c r="E63" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="F63" s="36" t="s">
+      <c r="F63" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="G63" s="41" t="s">
+      <c r="G63" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="H63" s="38"/>
+      <c r="H63" s="37"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3176,15 +3184,15 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1">
-      <c r="A64" s="17"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="42"/>
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
+      <c r="A64" s="16"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="41"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3205,26 +3213,26 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="59">
+      <c r="A65" s="64">
         <v>8</v>
       </c>
-      <c r="B65" s="62" t="s">
+      <c r="B65" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="21" t="s">
+      <c r="D65" s="26"/>
+      <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="56" t="s">
+      <c r="F65" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="G65" s="41" t="s">
+      <c r="G65" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H65" s="38"/>
+      <c r="H65" s="37"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3245,18 +3253,18 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="60"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="22" t="s">
+      <c r="A66" s="65"/>
+      <c r="B66" s="68"/>
+      <c r="C66" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="21" t="s">
+      <c r="D66" s="26"/>
+      <c r="E66" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F66" s="57"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="38"/>
+      <c r="F66" s="86"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="37"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -3277,18 +3285,18 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="60"/>
-      <c r="B67" s="63"/>
-      <c r="C67" s="22" t="s">
+      <c r="A67" s="65"/>
+      <c r="B67" s="68"/>
+      <c r="C67" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="21" t="s">
+      <c r="D67" s="26"/>
+      <c r="E67" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="57"/>
+      <c r="F67" s="86"/>
       <c r="G67" s="12"/>
-      <c r="H67" s="38"/>
+      <c r="H67" s="37"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -3309,14 +3317,14 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="61"/>
-      <c r="B68" s="64"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="58"/>
+      <c r="A68" s="66"/>
+      <c r="B68" s="69"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="87"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="38"/>
+      <c r="H68" s="37"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -3336,15 +3344,15 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.149999999999999" customHeight="1">
-      <c r="A69" s="17"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="42"/>
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+      <c r="A69" s="16"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="41"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -3368,19 +3376,19 @@
       <c r="A70" s="12">
         <v>9</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C70" s="22"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="31" t="s">
+      <c r="C70" s="21"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="F70" s="36" t="s">
+      <c r="F70" s="35" t="s">
         <v>97</v>
       </c>
       <c r="G70" s="12"/>
-      <c r="H70" s="38"/>
+      <c r="H70" s="37"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3402,6 +3410,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="D11:D29"/>
+    <mergeCell ref="F11:F29"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3418,22 +3442,6 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="D11:D29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
test cases ID's have been added to the RTM
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AyaMohamed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Project\Learning-hub\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
   <si>
     <t>Project Name:</t>
   </si>
@@ -424,6 +424,24 @@
   </si>
   <si>
     <t>resetPassword(email,password)</t>
+  </si>
+  <si>
+    <t>RM_1</t>
+  </si>
+  <si>
+    <t>RM_2</t>
+  </si>
+  <si>
+    <t>RM_3 , RM_4</t>
+  </si>
+  <si>
+    <t>RM_5 , RM_9 , RM_10 , RM_11 , RM_12 , RM_13</t>
+  </si>
+  <si>
+    <t>RM_6 , RM_7 , RM_14 , RM_15 , RM_16, RM_17 , RM_18 , RM_19 , RM_20 , RM_21</t>
+  </si>
+  <si>
+    <t>RM_8 , RM_22 , RM_23, RM_24 , RM_25</t>
   </si>
 </sst>
 </file>
@@ -701,7 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -854,14 +872,32 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,43 +917,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -941,11 +941,35 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1274,42 +1298,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="17.5"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="54.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="78.42578125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.28515625" style="5"/>
+    <col min="1" max="1" width="23.26953125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="48.26953125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="35.7265625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="54.26953125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="78.453125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="44.54296875" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="9.26953125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
       <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
+      <c r="C2" s="79"/>
       <c r="D2" s="13" t="s">
         <v>51</v>
       </c>
@@ -1330,10 +1354,10 @@
       <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="85"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="14">
         <v>1</v>
       </c>
@@ -1354,10 +1378,10 @@
       <c r="A4" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="86">
+      <c r="B4" s="80">
         <v>43470</v>
       </c>
-      <c r="C4" s="86"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -1376,8 +1400,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="43"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="14">
         <v>1.2</v>
       </c>
@@ -1431,22 +1455,22 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
-      <c r="A8" s="66">
+      <c r="A8" s="82">
         <v>1</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="81" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="67"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="69"/>
+      <c r="H8" s="84"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1466,19 +1490,19 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="66"/>
-      <c r="B9" s="65"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.65" customHeight="1">
+      <c r="A9" s="82"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="67"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="69"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="69"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1527,26 +1551,26 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="66">
+      <c r="A11" s="82">
         <v>2</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="81" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="67"/>
+      <c r="D11" s="89"/>
       <c r="E11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="G11" s="87" t="s">
+      <c r="G11" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="66"/>
+      <c r="H11" s="82"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1567,17 +1591,17 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="66"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="67"/>
+      <c r="D12" s="89"/>
       <c r="E12" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="71"/>
-      <c r="H12" s="66"/>
+      <c r="F12" s="86"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1598,16 +1622,16 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="66"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="67"/>
+      <c r="D13" s="89"/>
       <c r="E13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="71"/>
+      <c r="F13" s="86"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="3"/>
@@ -1630,16 +1654,16 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="66"/>
-      <c r="B14" s="65"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="67"/>
+      <c r="D14" s="89"/>
       <c r="E14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="71"/>
+      <c r="F14" s="86"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="3"/>
@@ -1662,16 +1686,16 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="66"/>
-      <c r="B15" s="65"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="67"/>
+      <c r="D15" s="89"/>
       <c r="E15" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="71"/>
+      <c r="F15" s="86"/>
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
       <c r="I15" s="3"/>
@@ -1694,14 +1718,14 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="66"/>
-      <c r="B16" s="65"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="67"/>
+      <c r="D16" s="89"/>
       <c r="E16" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="71"/>
+      <c r="F16" s="86"/>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="3"/>
@@ -1724,14 +1748,14 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="66"/>
-      <c r="B17" s="65"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="67"/>
+      <c r="D17" s="89"/>
       <c r="E17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="71"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38"/>
       <c r="I17" s="3"/>
@@ -1754,14 +1778,14 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="66"/>
-      <c r="B18" s="65"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="67"/>
+      <c r="D18" s="89"/>
       <c r="E18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="71"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="38"/>
       <c r="H18" s="38"/>
       <c r="I18" s="3"/>
@@ -1784,14 +1808,14 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="66"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="24"/>
-      <c r="D19" s="67"/>
+      <c r="D19" s="89"/>
       <c r="E19" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="71"/>
+      <c r="F19" s="86"/>
       <c r="G19" s="38"/>
       <c r="H19" s="38"/>
       <c r="I19" s="3"/>
@@ -1814,14 +1838,14 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="66"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="24"/>
-      <c r="D20" s="67"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="71"/>
+      <c r="F20" s="86"/>
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
       <c r="I20" s="3"/>
@@ -1844,14 +1868,14 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="66"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="81"/>
       <c r="C21" s="24"/>
-      <c r="D21" s="67"/>
+      <c r="D21" s="89"/>
       <c r="E21" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="71"/>
+      <c r="F21" s="86"/>
       <c r="G21" s="53" t="s">
         <v>119</v>
       </c>
@@ -1876,14 +1900,14 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="66"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="24"/>
-      <c r="D22" s="67"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="71"/>
+      <c r="F22" s="86"/>
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
       <c r="I22" s="3"/>
@@ -1906,14 +1930,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="66"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="67"/>
+      <c r="D23" s="89"/>
       <c r="E23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="71"/>
+      <c r="F23" s="86"/>
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
       <c r="I23" s="3"/>
@@ -1936,14 +1960,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="66"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="67"/>
+      <c r="D24" s="89"/>
       <c r="E24" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="71"/>
+      <c r="F24" s="86"/>
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
       <c r="I24" s="3"/>
@@ -1966,15 +1990,17 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="66"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="67"/>
+      <c r="D25" s="71" t="s">
+        <v>120</v>
+      </c>
       <c r="E25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="71"/>
-      <c r="G25" s="88" t="s">
+      <c r="F25" s="86"/>
+      <c r="G25" s="57" t="s">
         <v>116</v>
       </c>
       <c r="H25" s="38"/>
@@ -1998,14 +2024,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="66"/>
-      <c r="B26" s="65"/>
+      <c r="A26" s="82"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="67"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="71"/>
+      <c r="F26" s="86"/>
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
       <c r="I26" s="3"/>
@@ -2028,14 +2054,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="66"/>
-      <c r="B27" s="65"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="24"/>
-      <c r="D27" s="67"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="71"/>
+      <c r="F27" s="86"/>
       <c r="G27" s="38"/>
       <c r="H27" s="38"/>
       <c r="I27" s="3"/>
@@ -2058,14 +2084,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="66"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="67"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="71"/>
+      <c r="F28" s="86"/>
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
       <c r="I28" s="3"/>
@@ -2088,14 +2114,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="66"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="24"/>
-      <c r="D29" s="67"/>
+      <c r="D29" s="72"/>
       <c r="E29" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="71"/>
+      <c r="F29" s="86"/>
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
       <c r="I29" s="3"/>
@@ -2121,7 +2147,7 @@
       <c r="A30" s="12"/>
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
-      <c r="D30" s="27"/>
+      <c r="D30" s="72"/>
       <c r="E30" s="30" t="s">
         <v>67</v>
       </c>
@@ -2151,7 +2177,7 @@
       <c r="A31" s="12"/>
       <c r="B31" s="20"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="27"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="30" t="s">
         <v>68</v>
       </c>
@@ -2181,7 +2207,7 @@
       <c r="A32" s="12"/>
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
-      <c r="D32" s="27"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="30" t="s">
         <v>69</v>
       </c>
@@ -2207,11 +2233,13 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="33" spans="1:26" s="4" customFormat="1">
       <c r="A33" s="12"/>
       <c r="B33" s="20"/>
       <c r="C33" s="22"/>
-      <c r="D33" s="27"/>
+      <c r="D33" s="27" t="s">
+        <v>122</v>
+      </c>
       <c r="E33" s="30" t="s">
         <v>70</v>
       </c>
@@ -2237,11 +2265,13 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="52.5">
       <c r="A34" s="12"/>
       <c r="B34" s="20"/>
       <c r="C34" s="22"/>
-      <c r="D34" s="27"/>
+      <c r="D34" s="90" t="s">
+        <v>123</v>
+      </c>
       <c r="E34" s="30" t="s">
         <v>71</v>
       </c>
@@ -2267,11 +2297,13 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="112" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
-      <c r="D35" s="27"/>
+      <c r="D35" s="71" t="s">
+        <v>124</v>
+      </c>
       <c r="E35" s="30" t="s">
         <v>72</v>
       </c>
@@ -2297,11 +2329,11 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="36" spans="1:26" s="4" customFormat="1">
       <c r="A36" s="12"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="27"/>
+      <c r="D36" s="73"/>
       <c r="E36" s="30" t="s">
         <v>73</v>
       </c>
@@ -2327,11 +2359,13 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="52.5">
       <c r="A37" s="12"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
-      <c r="D37" s="27"/>
+      <c r="D37" s="27" t="s">
+        <v>125</v>
+      </c>
       <c r="E37" s="30" t="s">
         <v>74</v>
       </c>
@@ -2361,7 +2395,9 @@
       <c r="A38" s="12"/>
       <c r="B38" s="20"/>
       <c r="C38" s="22"/>
-      <c r="D38" s="27"/>
+      <c r="D38" s="27" t="s">
+        <v>121</v>
+      </c>
       <c r="E38" s="30" t="s">
         <v>102</v>
       </c>
@@ -2387,7 +2423,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1">
+    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.5" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="19"/>
       <c r="C39" s="23"/>
@@ -2429,7 +2465,7 @@
       <c r="E40" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="56" t="s">
+      <c r="F40" s="62" t="s">
         <v>92</v>
       </c>
       <c r="G40" s="12"/>
@@ -2463,7 +2499,7 @@
       <c r="E41" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="76"/>
+      <c r="F41" s="63"/>
       <c r="G41" s="12"/>
       <c r="H41" s="38"/>
       <c r="I41" s="3"/>
@@ -2495,7 +2531,7 @@
       <c r="E42" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="76"/>
+      <c r="F42" s="63"/>
       <c r="G42" s="12"/>
       <c r="H42" s="38"/>
       <c r="I42" s="3"/>
@@ -2525,7 +2561,7 @@
       <c r="E43" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="76"/>
+      <c r="F43" s="63"/>
       <c r="G43" s="12"/>
       <c r="H43" s="38"/>
       <c r="I43" s="3"/>
@@ -2557,7 +2593,7 @@
       <c r="E44" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="77"/>
+      <c r="F44" s="64"/>
       <c r="G44" s="12"/>
       <c r="H44" s="38"/>
       <c r="I44" s="3"/>
@@ -2611,7 +2647,7 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
+    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.65" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="19"/>
       <c r="C46" s="23"/>
@@ -2640,20 +2676,20 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="59">
+      <c r="A47" s="65">
         <v>4</v>
       </c>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="68" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="68"/>
+      <c r="D47" s="71"/>
       <c r="E47" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="56" t="s">
+      <c r="F47" s="62" t="s">
         <v>93</v>
       </c>
       <c r="G47" s="38" t="s">
@@ -2680,16 +2716,16 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="60"/>
-      <c r="B48" s="63"/>
+      <c r="A48" s="66"/>
+      <c r="B48" s="69"/>
       <c r="C48" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="78"/>
+      <c r="D48" s="72"/>
       <c r="E48" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="76"/>
+      <c r="F48" s="63"/>
       <c r="G48" s="39"/>
       <c r="H48" s="39"/>
       <c r="I48" s="9"/>
@@ -2712,14 +2748,14 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="63"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="69"/>
       <c r="C49" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="78"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="76"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="63"/>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
       <c r="I49" s="3"/>
@@ -2742,12 +2778,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="60"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="76"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="69"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="72"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="63"/>
       <c r="G50" s="38"/>
       <c r="H50" s="38"/>
       <c r="I50" s="3"/>
@@ -2770,12 +2806,12 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="61"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="77"/>
+      <c r="A51" s="67"/>
+      <c r="B51" s="70"/>
+      <c r="C51" s="75"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="64"/>
       <c r="G51" s="38"/>
       <c r="H51" s="38"/>
       <c r="I51" s="3"/>
@@ -2797,7 +2833,7 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
+    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.65" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="19"/>
       <c r="C52" s="23"/>
@@ -2826,10 +2862,10 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A53" s="66">
+      <c r="A53" s="82">
         <v>5</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="81" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="22" t="s">
@@ -2839,7 +2875,7 @@
       <c r="E53" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="56" t="s">
+      <c r="F53" s="62" t="s">
         <v>94</v>
       </c>
       <c r="G53" s="12"/>
@@ -2864,14 +2900,14 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="66"/>
-      <c r="B54" s="65"/>
+      <c r="A54" s="82"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="57"/>
+      <c r="F54" s="87"/>
       <c r="G54" s="41"/>
       <c r="H54" s="38"/>
       <c r="I54" s="3"/>
@@ -2894,14 +2930,14 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="66"/>
-      <c r="B55" s="65"/>
+      <c r="A55" s="82"/>
+      <c r="B55" s="81"/>
       <c r="C55" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="28"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="58"/>
+      <c r="F55" s="88"/>
       <c r="G55" s="12"/>
       <c r="H55" s="38"/>
       <c r="I55" s="3"/>
@@ -2923,7 +2959,7 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.649999999999999" customHeight="1">
       <c r="A56" s="17"/>
       <c r="B56" s="19"/>
       <c r="C56" s="23"/>
@@ -2952,18 +2988,18 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="66">
+      <c r="A57" s="82">
         <v>6</v>
       </c>
-      <c r="B57" s="65" t="s">
+      <c r="B57" s="81" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="24"/>
-      <c r="D57" s="67"/>
+      <c r="D57" s="83"/>
       <c r="E57" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F57" s="56" t="s">
+      <c r="F57" s="62" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="12"/>
@@ -2988,13 +3024,13 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="66"/>
-      <c r="B58" s="65"/>
-      <c r="D58" s="67"/>
+      <c r="A58" s="82"/>
+      <c r="B58" s="81"/>
+      <c r="D58" s="83"/>
       <c r="E58" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="57"/>
+      <c r="F58" s="87"/>
       <c r="G58" s="41"/>
       <c r="H58" s="38"/>
       <c r="I58" s="3"/>
@@ -3017,16 +3053,16 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="66"/>
-      <c r="B59" s="65"/>
+      <c r="A59" s="82"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="68"/>
+      <c r="D59" s="71"/>
       <c r="E59" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="58"/>
+      <c r="F59" s="88"/>
       <c r="G59" s="41"/>
       <c r="H59" s="38"/>
       <c r="I59" s="3"/>
@@ -3176,7 +3212,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1">
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.5" customHeight="1">
       <c r="A64" s="17"/>
       <c r="B64" s="19"/>
       <c r="C64" s="23"/>
@@ -3205,10 +3241,10 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="59">
+      <c r="A65" s="65">
         <v>8</v>
       </c>
-      <c r="B65" s="62" t="s">
+      <c r="B65" s="68" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="22" t="s">
@@ -3218,7 +3254,7 @@
       <c r="E65" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="56" t="s">
+      <c r="F65" s="62" t="s">
         <v>98</v>
       </c>
       <c r="G65" s="41" t="s">
@@ -3245,8 +3281,8 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="60"/>
-      <c r="B66" s="63"/>
+      <c r="A66" s="66"/>
+      <c r="B66" s="69"/>
       <c r="C66" s="22" t="s">
         <v>86</v>
       </c>
@@ -3254,7 +3290,7 @@
       <c r="E66" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F66" s="57"/>
+      <c r="F66" s="87"/>
       <c r="G66" s="41"/>
       <c r="H66" s="38"/>
       <c r="I66" s="3"/>
@@ -3277,8 +3313,8 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="60"/>
-      <c r="B67" s="63"/>
+      <c r="A67" s="66"/>
+      <c r="B67" s="69"/>
       <c r="C67" s="22" t="s">
         <v>85</v>
       </c>
@@ -3286,7 +3322,7 @@
       <c r="E67" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="57"/>
+      <c r="F67" s="87"/>
       <c r="G67" s="12"/>
       <c r="H67" s="38"/>
       <c r="I67" s="3"/>
@@ -3309,12 +3345,12 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="61"/>
-      <c r="B68" s="64"/>
+      <c r="A68" s="67"/>
+      <c r="B68" s="70"/>
       <c r="C68" s="22"/>
       <c r="D68" s="27"/>
       <c r="E68" s="21"/>
-      <c r="F68" s="58"/>
+      <c r="F68" s="88"/>
       <c r="G68" s="12"/>
       <c r="H68" s="38"/>
       <c r="I68" s="3"/>
@@ -3401,7 +3437,24 @@
       <c r="Z70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="F11:F29"/>
+    <mergeCell ref="D25:D32"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3418,22 +3471,6 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="D11:D29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
update RTM with article module testcase
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Project\Learning-hub\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
   <si>
     <t>Project Name:</t>
   </si>
@@ -442,6 +442,23 @@
   </si>
   <si>
     <t>RM_8 , RM_22 , RM_23, RM_24 , RM_25</t>
+  </si>
+  <si>
+    <t>AM_9</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5,AM_6,
+AM_7</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5 ,AM_6,AM_7</t>
+  </si>
+  <si>
+    <t>AM_4 ,AM_8</t>
   </si>
 </sst>
 </file>
@@ -572,7 +589,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +629,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,7 +742,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -884,76 +907,52 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -970,6 +969,58 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1298,42 +1349,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65:B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="17.5"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="48.26953125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="35.7265625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="54.26953125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="78.453125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="44.54296875" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.26953125" style="5"/>
+    <col min="1" max="1" width="23.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="54.28515625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="78.42578125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="89"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="13" t="s">
         <v>51</v>
       </c>
@@ -1354,10 +1405,10 @@
       <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="89"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="14">
         <v>1</v>
       </c>
@@ -1378,10 +1429,10 @@
       <c r="A4" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="90">
+      <c r="B4" s="82">
         <v>43470</v>
       </c>
-      <c r="C4" s="90"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -1400,8 +1451,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="43"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="81"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="14">
         <v>1.2</v>
       </c>
@@ -1455,22 +1506,22 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
-      <c r="A8" s="72">
+      <c r="A8" s="84">
         <v>1</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="83" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="73"/>
+      <c r="D8" s="85"/>
       <c r="E8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="74"/>
+      <c r="F8" s="86"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="74"/>
+      <c r="H8" s="86"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1490,19 +1541,19 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.65" customHeight="1">
-      <c r="A9" s="72"/>
-      <c r="B9" s="71"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A9" s="84"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="73"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="74"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="74"/>
+      <c r="H9" s="86"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1551,10 +1602,10 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="72">
+      <c r="A11" s="84">
         <v>2</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="83" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="22" t="s">
@@ -1564,13 +1615,13 @@
       <c r="E11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="87" t="s">
         <v>91</v>
       </c>
       <c r="G11" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="72"/>
+      <c r="H11" s="84"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1591,8 +1642,8 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="72"/>
-      <c r="B12" s="71"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
@@ -1600,8 +1651,8 @@
       <c r="E12" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="76"/>
-      <c r="H12" s="72"/>
+      <c r="F12" s="88"/>
+      <c r="H12" s="84"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1622,8 +1673,8 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="72"/>
-      <c r="B13" s="71"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="22" t="s">
         <v>16</v>
       </c>
@@ -1631,7 +1682,7 @@
       <c r="E13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="76"/>
+      <c r="F13" s="88"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="3"/>
@@ -1654,8 +1705,8 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="72"/>
-      <c r="B14" s="71"/>
+      <c r="A14" s="84"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="22" t="s">
         <v>87</v>
       </c>
@@ -1663,7 +1714,7 @@
       <c r="E14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="76"/>
+      <c r="F14" s="88"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="3"/>
@@ -1686,8 +1737,8 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="72"/>
-      <c r="B15" s="71"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="22" t="s">
         <v>84</v>
       </c>
@@ -1695,7 +1746,7 @@
       <c r="E15" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="76"/>
+      <c r="F15" s="88"/>
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
       <c r="I15" s="3"/>
@@ -1718,14 +1769,14 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="72"/>
-      <c r="B16" s="71"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="24"/>
       <c r="D16" s="58"/>
       <c r="E16" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="76"/>
+      <c r="F16" s="88"/>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="3"/>
@@ -1748,14 +1799,14 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="72"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="24"/>
       <c r="D17" s="58"/>
       <c r="E17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="76"/>
+      <c r="F17" s="88"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38"/>
       <c r="I17" s="3"/>
@@ -1778,14 +1829,14 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="72"/>
-      <c r="B18" s="71"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="24"/>
       <c r="D18" s="58"/>
       <c r="E18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="76"/>
+      <c r="F18" s="88"/>
       <c r="G18" s="38"/>
       <c r="H18" s="38"/>
       <c r="I18" s="3"/>
@@ -1808,14 +1859,14 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="72"/>
-      <c r="B19" s="71"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="24"/>
       <c r="D19" s="58"/>
       <c r="E19" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="76"/>
+      <c r="F19" s="88"/>
       <c r="G19" s="38"/>
       <c r="H19" s="38"/>
       <c r="I19" s="3"/>
@@ -1838,14 +1889,14 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="72"/>
-      <c r="B20" s="71"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="83"/>
       <c r="C20" s="24"/>
       <c r="D20" s="58"/>
       <c r="E20" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="76"/>
+      <c r="F20" s="88"/>
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
       <c r="I20" s="3"/>
@@ -1868,14 +1919,14 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="71"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="83"/>
       <c r="C21" s="24"/>
       <c r="D21" s="58"/>
       <c r="E21" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="76"/>
+      <c r="F21" s="88"/>
       <c r="G21" s="53" t="s">
         <v>119</v>
       </c>
@@ -1900,14 +1951,14 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="72"/>
-      <c r="B22" s="71"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="24"/>
       <c r="D22" s="58"/>
       <c r="E22" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="76"/>
+      <c r="F22" s="88"/>
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
       <c r="I22" s="3"/>
@@ -1930,14 +1981,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="72"/>
-      <c r="B23" s="71"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="24"/>
       <c r="D23" s="58"/>
       <c r="E23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="76"/>
+      <c r="F23" s="88"/>
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
       <c r="I23" s="3"/>
@@ -1960,14 +2011,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="72"/>
-      <c r="B24" s="71"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="24"/>
       <c r="D24" s="58"/>
       <c r="E24" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="76"/>
+      <c r="F24" s="88"/>
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
       <c r="I24" s="3"/>
@@ -1990,16 +2041,16 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="71"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="83"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="73" t="s">
         <v>120</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="76"/>
+      <c r="F25" s="88"/>
       <c r="G25" s="57" t="s">
         <v>116</v>
       </c>
@@ -2024,14 +2075,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="72"/>
-      <c r="B26" s="71"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="83"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="77"/>
+      <c r="D26" s="74"/>
       <c r="E26" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="76"/>
+      <c r="F26" s="88"/>
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
       <c r="I26" s="3"/>
@@ -2054,14 +2105,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="72"/>
-      <c r="B27" s="71"/>
+      <c r="A27" s="84"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="24"/>
-      <c r="D27" s="77"/>
+      <c r="D27" s="74"/>
       <c r="E27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="76"/>
+      <c r="F27" s="88"/>
       <c r="G27" s="38"/>
       <c r="H27" s="38"/>
       <c r="I27" s="3"/>
@@ -2084,14 +2135,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="72"/>
-      <c r="B28" s="71"/>
+      <c r="A28" s="84"/>
+      <c r="B28" s="83"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="77"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="76"/>
+      <c r="F28" s="88"/>
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
       <c r="I28" s="3"/>
@@ -2114,14 +2165,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="72"/>
-      <c r="B29" s="71"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="83"/>
       <c r="C29" s="24"/>
-      <c r="D29" s="77"/>
+      <c r="D29" s="74"/>
       <c r="E29" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="76"/>
+      <c r="F29" s="88"/>
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
       <c r="I29" s="3"/>
@@ -2147,7 +2198,7 @@
       <c r="A30" s="12"/>
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
-      <c r="D30" s="77"/>
+      <c r="D30" s="74"/>
       <c r="E30" s="30" t="s">
         <v>67</v>
       </c>
@@ -2177,7 +2228,7 @@
       <c r="A31" s="12"/>
       <c r="B31" s="20"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="77"/>
+      <c r="D31" s="74"/>
       <c r="E31" s="30" t="s">
         <v>68</v>
       </c>
@@ -2207,7 +2258,7 @@
       <c r="A32" s="12"/>
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
-      <c r="D32" s="61"/>
+      <c r="D32" s="75"/>
       <c r="E32" s="30" t="s">
         <v>69</v>
       </c>
@@ -2265,7 +2316,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="52.5">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="54">
       <c r="A34" s="12"/>
       <c r="B34" s="20"/>
       <c r="C34" s="22"/>
@@ -2297,11 +2348,11 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="112" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="111.95" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="73" t="s">
         <v>124</v>
       </c>
       <c r="E35" s="30" t="s">
@@ -2333,7 +2384,7 @@
       <c r="A36" s="12"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="61"/>
+      <c r="D36" s="75"/>
       <c r="E36" s="30" t="s">
         <v>73</v>
       </c>
@@ -2359,7 +2410,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="52.5">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="54">
       <c r="A37" s="12"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
@@ -2423,7 +2474,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.5" customHeight="1">
+    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="19"/>
       <c r="C39" s="23"/>
@@ -2465,7 +2516,7 @@
       <c r="E40" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="62" t="s">
+      <c r="F40" s="64" t="s">
         <v>92</v>
       </c>
       <c r="G40" s="12"/>
@@ -2499,7 +2550,7 @@
       <c r="E41" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="82"/>
+      <c r="F41" s="65"/>
       <c r="G41" s="12"/>
       <c r="H41" s="38"/>
       <c r="I41" s="3"/>
@@ -2531,7 +2582,7 @@
       <c r="E42" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="82"/>
+      <c r="F42" s="65"/>
       <c r="G42" s="12"/>
       <c r="H42" s="38"/>
       <c r="I42" s="3"/>
@@ -2561,7 +2612,7 @@
       <c r="E43" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="82"/>
+      <c r="F43" s="65"/>
       <c r="G43" s="12"/>
       <c r="H43" s="38"/>
       <c r="I43" s="3"/>
@@ -2583,37 +2634,39 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A44" s="12"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="22" t="s">
+    <row r="44" spans="1:26" s="97" customFormat="1" ht="85.5" customHeight="1">
+      <c r="A44" s="91"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="22"/>
-      <c r="E44" s="31" t="s">
+      <c r="D44" s="93" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="83"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="95"/>
+      <c r="I44" s="96"/>
+      <c r="J44" s="96"/>
+      <c r="K44" s="96"/>
+      <c r="L44" s="96"/>
+      <c r="M44" s="96"/>
+      <c r="N44" s="96"/>
+      <c r="O44" s="96"/>
+      <c r="P44" s="96"/>
+      <c r="Q44" s="96"/>
+      <c r="R44" s="96"/>
+      <c r="S44" s="96"/>
+      <c r="T44" s="96"/>
+      <c r="U44" s="96"/>
+      <c r="V44" s="96"/>
+      <c r="W44" s="96"/>
+      <c r="X44" s="96"/>
+      <c r="Y44" s="96"/>
+      <c r="Z44" s="96"/>
     </row>
     <row r="45" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A45" s="12"/>
@@ -2647,7 +2700,7 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.65" customHeight="1">
+    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="19"/>
       <c r="C46" s="23"/>
@@ -2676,20 +2729,20 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="65">
+      <c r="A47" s="67">
         <v>4</v>
       </c>
-      <c r="B47" s="68" t="s">
+      <c r="B47" s="70" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="60"/>
+      <c r="D47" s="73"/>
       <c r="E47" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="62" t="s">
+      <c r="F47" s="64" t="s">
         <v>93</v>
       </c>
       <c r="G47" s="38" t="s">
@@ -2716,16 +2769,16 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="66"/>
-      <c r="B48" s="69"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="71"/>
       <c r="C48" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="77"/>
+      <c r="D48" s="74"/>
       <c r="E48" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="82"/>
+      <c r="F48" s="65"/>
       <c r="G48" s="39"/>
       <c r="H48" s="39"/>
       <c r="I48" s="9"/>
@@ -2748,14 +2801,14 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="66"/>
-      <c r="B49" s="69"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="71"/>
       <c r="C49" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="77"/>
-      <c r="E49" s="86"/>
-      <c r="F49" s="82"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="65"/>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
       <c r="I49" s="3"/>
@@ -2778,12 +2831,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="66"/>
-      <c r="B50" s="69"/>
-      <c r="C50" s="84"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="82"/>
+      <c r="A50" s="68"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="79"/>
+      <c r="F50" s="65"/>
       <c r="G50" s="38"/>
       <c r="H50" s="38"/>
       <c r="I50" s="3"/>
@@ -2806,12 +2859,12 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="67"/>
-      <c r="B51" s="70"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="88"/>
-      <c r="F51" s="83"/>
+      <c r="A51" s="69"/>
+      <c r="B51" s="72"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="66"/>
       <c r="G51" s="38"/>
       <c r="H51" s="38"/>
       <c r="I51" s="3"/>
@@ -2833,7 +2886,7 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.65" customHeight="1">
+    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="19"/>
       <c r="C52" s="23"/>
@@ -2862,10 +2915,10 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A53" s="72">
+      <c r="A53" s="84">
         <v>5</v>
       </c>
-      <c r="B53" s="71" t="s">
+      <c r="B53" s="83" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="22" t="s">
@@ -2875,7 +2928,7 @@
       <c r="E53" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="62" t="s">
+      <c r="F53" s="64" t="s">
         <v>94</v>
       </c>
       <c r="G53" s="12"/>
@@ -2900,14 +2953,14 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="72"/>
-      <c r="B54" s="71"/>
+      <c r="A54" s="84"/>
+      <c r="B54" s="83"/>
       <c r="C54" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="63"/>
+      <c r="F54" s="89"/>
       <c r="G54" s="41"/>
       <c r="H54" s="38"/>
       <c r="I54" s="3"/>
@@ -2930,14 +2983,14 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="72"/>
-      <c r="B55" s="71"/>
+      <c r="A55" s="84"/>
+      <c r="B55" s="83"/>
       <c r="C55" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="28"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="64"/>
+      <c r="F55" s="90"/>
       <c r="G55" s="12"/>
       <c r="H55" s="38"/>
       <c r="I55" s="3"/>
@@ -2959,7 +3012,7 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.649999999999999" customHeight="1">
+    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
       <c r="A56" s="17"/>
       <c r="B56" s="19"/>
       <c r="C56" s="23"/>
@@ -2988,18 +3041,18 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="72">
+      <c r="A57" s="84">
         <v>6</v>
       </c>
-      <c r="B57" s="71" t="s">
+      <c r="B57" s="83" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="24"/>
-      <c r="D57" s="73"/>
+      <c r="D57" s="85"/>
       <c r="E57" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F57" s="62" t="s">
+      <c r="F57" s="64" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="12"/>
@@ -3024,13 +3077,13 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="72"/>
-      <c r="B58" s="71"/>
-      <c r="D58" s="73"/>
+      <c r="A58" s="84"/>
+      <c r="B58" s="83"/>
+      <c r="D58" s="85"/>
       <c r="E58" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="63"/>
+      <c r="F58" s="89"/>
       <c r="G58" s="41"/>
       <c r="H58" s="38"/>
       <c r="I58" s="3"/>
@@ -3053,16 +3106,16 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="72"/>
-      <c r="B59" s="71"/>
+      <c r="A59" s="84"/>
+      <c r="B59" s="83"/>
       <c r="C59" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="60"/>
+      <c r="D59" s="73"/>
       <c r="E59" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="64"/>
+      <c r="F59" s="90"/>
       <c r="G59" s="41"/>
       <c r="H59" s="38"/>
       <c r="I59" s="3"/>
@@ -3212,7 +3265,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.5" customHeight="1">
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1">
       <c r="A64" s="17"/>
       <c r="B64" s="19"/>
       <c r="C64" s="23"/>
@@ -3240,117 +3293,123 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="65">
+    <row r="65" spans="1:26" s="97" customFormat="1" ht="86.25" customHeight="1">
+      <c r="A65" s="67">
         <v>8</v>
       </c>
-      <c r="B65" s="68" t="s">
+      <c r="B65" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="21" t="s">
+      <c r="D65" s="98" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="62" t="s">
+      <c r="F65" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="G65" s="41" t="s">
+      <c r="G65" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="H65" s="38"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
-      <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
-      <c r="X65" s="3"/>
-      <c r="Y65" s="3"/>
-      <c r="Z65" s="3"/>
-    </row>
-    <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="66"/>
-      <c r="B66" s="69"/>
-      <c r="C66" s="22" t="s">
+      <c r="H65" s="95"/>
+      <c r="I65" s="96"/>
+      <c r="J65" s="96"/>
+      <c r="K65" s="96"/>
+      <c r="L65" s="96"/>
+      <c r="M65" s="96"/>
+      <c r="N65" s="96"/>
+      <c r="O65" s="96"/>
+      <c r="P65" s="96"/>
+      <c r="Q65" s="96"/>
+      <c r="R65" s="96"/>
+      <c r="S65" s="96"/>
+      <c r="T65" s="96"/>
+      <c r="U65" s="96"/>
+      <c r="V65" s="96"/>
+      <c r="W65" s="96"/>
+      <c r="X65" s="96"/>
+      <c r="Y65" s="96"/>
+      <c r="Z65" s="96"/>
+    </row>
+    <row r="66" spans="1:26" s="97" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A66" s="68"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="21" t="s">
+      <c r="D66" s="98" t="s">
+        <v>129</v>
+      </c>
+      <c r="E66" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F66" s="63"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="O66" s="3"/>
-      <c r="P66" s="3"/>
-      <c r="Q66" s="3"/>
-      <c r="R66" s="3"/>
-      <c r="S66" s="3"/>
-      <c r="T66" s="3"/>
-      <c r="U66" s="3"/>
-      <c r="V66" s="3"/>
-      <c r="W66" s="3"/>
-      <c r="X66" s="3"/>
-      <c r="Y66" s="3"/>
-      <c r="Z66" s="3"/>
-    </row>
-    <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="66"/>
-      <c r="B67" s="69"/>
-      <c r="C67" s="22" t="s">
+      <c r="F66" s="89"/>
+      <c r="G66" s="100"/>
+      <c r="H66" s="95"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="96"/>
+      <c r="M66" s="96"/>
+      <c r="N66" s="96"/>
+      <c r="O66" s="96"/>
+      <c r="P66" s="96"/>
+      <c r="Q66" s="96"/>
+      <c r="R66" s="96"/>
+      <c r="S66" s="96"/>
+      <c r="T66" s="96"/>
+      <c r="U66" s="96"/>
+      <c r="V66" s="96"/>
+      <c r="W66" s="96"/>
+      <c r="X66" s="96"/>
+      <c r="Y66" s="96"/>
+      <c r="Z66" s="96"/>
+    </row>
+    <row r="67" spans="1:26" s="97" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A67" s="68"/>
+      <c r="B67" s="71"/>
+      <c r="C67" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="21" t="s">
+      <c r="D67" s="98" t="s">
+        <v>126</v>
+      </c>
+      <c r="E67" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="63"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
-      <c r="Y67" s="3"/>
-      <c r="Z67" s="3"/>
+      <c r="F67" s="89"/>
+      <c r="G67" s="91"/>
+      <c r="H67" s="95"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="96"/>
+      <c r="K67" s="96"/>
+      <c r="L67" s="96"/>
+      <c r="M67" s="96"/>
+      <c r="N67" s="96"/>
+      <c r="O67" s="96"/>
+      <c r="P67" s="96"/>
+      <c r="Q67" s="96"/>
+      <c r="R67" s="96"/>
+      <c r="S67" s="96"/>
+      <c r="T67" s="96"/>
+      <c r="U67" s="96"/>
+      <c r="V67" s="96"/>
+      <c r="W67" s="96"/>
+      <c r="X67" s="96"/>
+      <c r="Y67" s="96"/>
+      <c r="Z67" s="96"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="67"/>
-      <c r="B68" s="70"/>
+      <c r="A68" s="69"/>
+      <c r="B68" s="72"/>
       <c r="C68" s="22"/>
       <c r="D68" s="27"/>
       <c r="E68" s="21"/>
-      <c r="F68" s="64"/>
+      <c r="F68" s="90"/>
       <c r="G68" s="12"/>
       <c r="H68" s="38"/>
       <c r="I68" s="3"/>
@@ -3438,6 +3497,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="F11:F29"/>
+    <mergeCell ref="D25:D32"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3454,23 +3530,6 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="D25:D32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
added function names in RTM
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Edit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="23004" windowHeight="7404"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23010" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="163">
   <si>
     <t>Project Name:</t>
   </si>
@@ -356,10 +356,6 @@
     <t>Lhub_SRS_2.4.3.11</t>
   </si>
   <si>
-    <t>Lhub_SRS_2.4.4.1
-Lhub_SRS_2.4.4.2</t>
-  </si>
-  <si>
     <t>Lhub_SRS_2.4.2.14</t>
   </si>
   <si>
@@ -397,21 +393,6 @@
   </si>
   <si>
     <t>Lhub_SRS_2.4.3.13</t>
-  </si>
-  <si>
-    <t>login_user(string username , string password)</t>
-  </si>
-  <si>
-    <t>signup_user(string username, string password, string fname, string lname, string email)</t>
-  </si>
-  <si>
-    <t>followCategory(username, categoryName)</t>
-  </si>
-  <si>
-    <t>reviewArticle(option , author, title)</t>
-  </si>
-  <si>
-    <t>resetPassword(email,password)</t>
   </si>
   <si>
     <t>update the SRS IDs column according to SRS document as SRS login module was updated</t>
@@ -477,6 +458,120 @@
 HM_14
 HM_15
 HM_16</t>
+  </si>
+  <si>
+    <t>UserClass.cs.login_user(string username , string password)</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx(usernameTxt)</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx(userNameRequiredValidator)</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx(passwordTxt)</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx(passwordRequiredValidator)</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx</t>
+  </si>
+  <si>
+    <t>UserClass.cs.resetPassword(email,password)</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx.loginBtn</t>
+  </si>
+  <si>
+    <t>HomePage.aspx</t>
+  </si>
+  <si>
+    <t>LoginPage.aspx.newAccountLink</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.usernametxt</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.FirstNametxt</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.LastNametxt</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.Emailtxt</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.passwordtxt</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.Confrim_passtxt</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.SignUpBtn</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.userNameExpressionValidator</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.passwordExpressionValidator</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.emailExpressionValidator</t>
+  </si>
+  <si>
+    <t>SignUpPage.aspx.userNameRequiredValidator
+, SignUpPage.aspx.passwordRequiredValidator
+, SignUpPage.aspx.confirmPasswordRequiredValidator
+, SignUpPage.aspx.emailRequiredValidator</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.11</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.12</t>
+  </si>
+  <si>
+    <t>HomePage.aspx.addBtn
+UploadArticlesPage.aspx</t>
+  </si>
+  <si>
+    <t>UploadArticlesPage.aspx</t>
+  </si>
+  <si>
+    <t>AdminClass.cs.reviewArticle(string option,string author ,string title)
+AdminRequests2.aspx</t>
+  </si>
+  <si>
+    <t>UserClass.searchArticle(string keyword)
+HomePage.aspx.srchtxt</t>
+  </si>
+  <si>
+    <t>SearchResultsPage.aspx</t>
+  </si>
+  <si>
+    <t>UserClass.cs.followCategory(username, categoryName)
+UserClass.cs.unfollowCategory(username , categoryName)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lhub_SRS_2.4.4.1
+</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.4.2</t>
+  </si>
+  <si>
+    <t>AdminRequests.aspx.reviewArticle(option , author, title)
+AdminClass.cs.reviewArtice(option , author,title)</t>
+  </si>
+  <si>
+    <t>AdminRequests.aspx.requestsGrid</t>
+  </si>
+  <si>
+    <t>CategoryPage.aspx</t>
   </si>
 </sst>
 </file>
@@ -486,7 +581,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,7 +856,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -896,15 +991,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -914,12 +1003,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -932,6 +1015,78 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -944,34 +1099,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,47 +1126,29 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1364,66 +1477,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.296875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="30.3984375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="48.296875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="28.796875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="35.59765625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="54.296875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="78.3984375" style="17" customWidth="1"/>
+    <col min="1" max="1" width="23.25" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="48.25" style="17" customWidth="1"/>
+    <col min="4" max="4" width="28.75" style="17" customWidth="1"/>
+    <col min="5" max="5" width="35.625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="54.25" style="20" customWidth="1"/>
+    <col min="7" max="7" width="78.375" style="17" customWidth="1"/>
     <col min="8" max="8" width="44.5" style="17" customWidth="1"/>
-    <col min="9" max="16384" width="9.296875" style="5"/>
+    <col min="9" max="16384" width="9.25" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.95" customHeight="1">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="D1" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
       <c r="G1" s="43"/>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="59" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="95"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1431,7 +1544,7 @@
         <v>43588</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="45" t="s">
         <v>54</v>
@@ -1440,14 +1553,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="84">
+        <v>103</v>
+      </c>
+      <c r="B4" s="96">
         <v>43470</v>
       </c>
-      <c r="C4" s="84"/>
+      <c r="C4" s="96"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1455,7 +1568,7 @@
         <v>43592</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="45" t="s">
         <v>76</v>
@@ -1464,10 +1577,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+    <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="42"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
@@ -1475,19 +1588,19 @@
         <v>43601</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.2" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="13">
         <v>1.3</v>
       </c>
@@ -1495,14 +1608,14 @@
         <v>43608</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>116</v>
+        <v>101</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>110</v>
       </c>
       <c r="H6" s="45"/>
     </row>
-    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1">
+    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1528,23 +1641,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
-      <c r="A8" s="86">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="74">
         <v>1</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="73" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="56"/>
       <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="87"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="36"/>
-      <c r="H8" s="87"/>
+      <c r="H8" s="77"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1564,19 +1677,19 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="86"/>
-      <c r="B9" s="85"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="74"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="60"/>
+      <c r="D9" s="56"/>
       <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="87"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="87"/>
+      <c r="H9" s="77"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1596,7 +1709,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.95" customHeight="1">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="18"/>
       <c r="C10" s="22"/>
@@ -1624,29 +1737,29 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="86">
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="59">
         <v>2</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="58" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="29" t="s">
+      <c r="D11" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="86"/>
+      <c r="G11" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="74"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1666,20 +1779,23 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="86"/>
-      <c r="B12" s="85"/>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="29" t="s">
+      <c r="D12" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="89"/>
-      <c r="H12" s="86"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="74"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1699,20 +1815,20 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="86"/>
-      <c r="B13" s="85"/>
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="59"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="29" t="s">
+      <c r="D13" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="89"/>
-      <c r="G13" s="37"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="104"/>
       <c r="H13" s="37"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1733,20 +1849,22 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="86"/>
-      <c r="B14" s="85"/>
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="29" t="s">
+      <c r="D14" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="89"/>
-      <c r="G14" s="37"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="20" t="s">
+        <v>130</v>
+      </c>
       <c r="H14" s="37"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1767,20 +1885,22 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="86"/>
-      <c r="B15" s="85"/>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="29" t="s">
+      <c r="D15" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="89"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="20" t="s">
+        <v>131</v>
+      </c>
       <c r="H15" s="37"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1801,18 +1921,20 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="86"/>
-      <c r="B16" s="85"/>
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="29" t="s">
+      <c r="D16" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="89"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="40" t="s">
+        <v>132</v>
+      </c>
       <c r="H16" s="37"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1833,18 +1955,20 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="86"/>
-      <c r="B17" s="85"/>
+    <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="23"/>
-      <c r="D17" s="60" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="29" t="s">
+      <c r="D17" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="89"/>
-      <c r="G17" s="37"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="40" t="s">
+        <v>133</v>
+      </c>
       <c r="H17" s="37"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1865,18 +1989,20 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="86"/>
-      <c r="B18" s="85"/>
+    <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="59"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="23"/>
-      <c r="D18" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="29" t="s">
+      <c r="D18" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="89"/>
-      <c r="G18" s="37"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="53" t="s">
+        <v>128</v>
+      </c>
       <c r="H18" s="37"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1897,18 +2023,20 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="86"/>
-      <c r="B19" s="85"/>
+    <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="59"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="23"/>
-      <c r="D19" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="29" t="s">
+      <c r="D19" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="89"/>
-      <c r="G19" s="37"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="40" t="s">
+        <v>134</v>
+      </c>
       <c r="H19" s="37"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -1929,18 +2057,20 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="86"/>
-      <c r="B20" s="85"/>
+    <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="23"/>
-      <c r="D20" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="57" t="s">
+      <c r="D20" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="89"/>
-      <c r="G20" s="37"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="40" t="s">
+        <v>135</v>
+      </c>
       <c r="H20" s="37"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1961,15 +2091,17 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="86"/>
-      <c r="B21" s="85"/>
+    <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="59"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="23"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="52" t="s">
-        <v>115</v>
+      <c r="D21" s="56"/>
+      <c r="E21" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="79"/>
+      <c r="G21" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H21" s="37"/>
       <c r="I21" s="3"/>
@@ -1991,14 +2123,18 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="86"/>
-      <c r="B22" s="85"/>
+    <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="59"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="23"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="37"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="79"/>
+      <c r="G22" s="97" t="s">
+        <v>137</v>
+      </c>
       <c r="H22" s="37"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -2019,14 +2155,14 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="86"/>
-      <c r="B23" s="85"/>
+    <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="59"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="37"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="98"/>
       <c r="H23" s="37"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -2047,14 +2183,18 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="86"/>
-      <c r="B24" s="85"/>
+    <row r="24" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="59"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="23"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="37"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="79"/>
+      <c r="G24" s="99" t="s">
+        <v>137</v>
+      </c>
       <c r="H24" s="37"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -2075,17 +2215,17 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="86"/>
-      <c r="B25" s="85"/>
+    <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="59"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="89"/>
-      <c r="G25" s="56" t="s">
-        <v>112</v>
+      <c r="D25" s="56"/>
+      <c r="E25" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="79"/>
+      <c r="G25" s="100" t="s">
+        <v>138</v>
       </c>
       <c r="H25" s="37"/>
       <c r="I25" s="3"/>
@@ -2107,16 +2247,18 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="86"/>
-      <c r="B26" s="85"/>
+    <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="59"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="23"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="89"/>
-      <c r="G26" s="37"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="79"/>
+      <c r="G26" s="40" t="s">
+        <v>139</v>
+      </c>
       <c r="H26" s="37"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -2137,16 +2279,18 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="86"/>
-      <c r="B27" s="85"/>
+    <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="59"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="23"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="89"/>
-      <c r="G27" s="37"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="79"/>
+      <c r="G27" s="40" t="s">
+        <v>140</v>
+      </c>
       <c r="H27" s="37"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -2167,16 +2311,18 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="86"/>
-      <c r="B28" s="85"/>
+    <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="59"/>
+      <c r="B28" s="58"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="89"/>
-      <c r="G28" s="37"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="79"/>
+      <c r="G28" s="40" t="s">
+        <v>141</v>
+      </c>
       <c r="H28" s="37"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -2197,16 +2343,18 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="86"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="89"/>
-      <c r="G29" s="37"/>
+    <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="33"/>
+      <c r="G29" s="40" t="s">
+        <v>142</v>
+      </c>
       <c r="H29" s="37"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -2227,16 +2375,18 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="19"/>
       <c r="C30" s="21"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="29" t="s">
-        <v>63</v>
+      <c r="E30" s="60" t="s">
+        <v>64</v>
       </c>
       <c r="F30" s="33"/>
-      <c r="G30" s="37"/>
+      <c r="G30" s="40" t="s">
+        <v>143</v>
+      </c>
       <c r="H30" s="37"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -2257,16 +2407,18 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="19"/>
       <c r="C31" s="21"/>
       <c r="D31" s="26"/>
-      <c r="E31" s="29" t="s">
-        <v>64</v>
+      <c r="E31" s="60" t="s">
+        <v>65</v>
       </c>
       <c r="F31" s="33"/>
-      <c r="G31" s="37"/>
+      <c r="G31" s="40" t="s">
+        <v>144</v>
+      </c>
       <c r="H31" s="37"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -2287,16 +2439,18 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="19"/>
       <c r="C32" s="21"/>
       <c r="D32" s="26"/>
-      <c r="E32" s="29" t="s">
-        <v>65</v>
+      <c r="E32" s="60" t="s">
+        <v>66</v>
       </c>
       <c r="F32" s="33"/>
-      <c r="G32" s="37"/>
+      <c r="G32" s="40" t="s">
+        <v>145</v>
+      </c>
       <c r="H32" s="37"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -2317,16 +2471,18 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
       <c r="B33" s="19"/>
       <c r="C33" s="21"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="29" t="s">
-        <v>66</v>
+      <c r="E33" s="60" t="s">
+        <v>67</v>
       </c>
       <c r="F33" s="33"/>
-      <c r="G33" s="37"/>
+      <c r="G33" s="40" t="s">
+        <v>146</v>
+      </c>
       <c r="H33" s="37"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -2347,16 +2503,18 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
       <c r="B34" s="19"/>
       <c r="C34" s="21"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="29" t="s">
-        <v>67</v>
+      <c r="E34" s="60" t="s">
+        <v>68</v>
       </c>
       <c r="F34" s="33"/>
-      <c r="G34" s="37"/>
+      <c r="G34" s="40" t="s">
+        <v>147</v>
+      </c>
       <c r="H34" s="37"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -2377,16 +2535,18 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
       <c r="B35" s="19"/>
       <c r="C35" s="21"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="29" t="s">
-        <v>68</v>
+      <c r="E35" s="60" t="s">
+        <v>69</v>
       </c>
       <c r="F35" s="33"/>
-      <c r="G35" s="37"/>
+      <c r="G35" s="40" t="s">
+        <v>147</v>
+      </c>
       <c r="H35" s="37"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -2407,16 +2567,18 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.95" customHeight="1">
+    <row r="36" spans="1:26" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
       <c r="B36" s="19"/>
       <c r="C36" s="21"/>
       <c r="D36" s="26"/>
-      <c r="E36" s="29" t="s">
-        <v>69</v>
+      <c r="E36" s="60" t="s">
+        <v>70</v>
       </c>
       <c r="F36" s="33"/>
-      <c r="G36" s="37"/>
+      <c r="G36" s="100" t="s">
+        <v>148</v>
+      </c>
       <c r="H36" s="37"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -2437,16 +2599,18 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="19"/>
       <c r="C37" s="21"/>
       <c r="D37" s="26"/>
-      <c r="E37" s="29" t="s">
-        <v>70</v>
+      <c r="E37" s="60" t="s">
+        <v>97</v>
       </c>
       <c r="F37" s="33"/>
-      <c r="G37" s="38"/>
+      <c r="G37" s="101" t="s">
+        <v>149</v>
+      </c>
       <c r="H37" s="37"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
@@ -2467,84 +2631,92 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38" s="33"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-    </row>
-    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.4" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6"/>
-    </row>
-    <row r="40" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A40" s="12">
+    <row r="38" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="16"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="6"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="6"/>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
+    </row>
+    <row r="39" spans="1:26" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12">
         <v>3</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B39" s="19" t="s">
         <v>32</v>
       </c>
+      <c r="C39" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="102" t="s">
+        <v>152</v>
+      </c>
+      <c r="H39" s="37"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+    </row>
+    <row r="40" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="96" t="s">
-        <v>125</v>
+        <v>18</v>
+      </c>
+      <c r="D40" s="61" t="s">
+        <v>120</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="G40" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="F40" s="86"/>
+      <c r="G40" s="40" t="s">
+        <v>153</v>
+      </c>
       <c r="H40" s="37"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -2565,20 +2737,22 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="41" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
       <c r="B41" s="19"/>
       <c r="C41" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="96" t="s">
-        <v>126</v>
+        <v>19</v>
+      </c>
+      <c r="D41" s="62" t="s">
+        <v>121</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="67"/>
-      <c r="G41" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="F41" s="86"/>
+      <c r="G41" s="40" t="s">
+        <v>153</v>
+      </c>
       <c r="H41" s="37"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -2599,20 +2773,18 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1">
+    <row r="42" spans="1:26" s="8" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="19"/>
-      <c r="C42" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="97" t="s">
-        <v>127</v>
+      <c r="C42" s="21"/>
+      <c r="D42" s="62" t="s">
+        <v>121</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" s="67"/>
-      <c r="G42" s="12"/>
+        <v>105</v>
+      </c>
+      <c r="F42" s="86"/>
+      <c r="G42" s="40"/>
       <c r="H42" s="37"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -2633,18 +2805,20 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="8" customFormat="1" ht="59.4" customHeight="1">
+    <row r="43" spans="1:26" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="19"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="97" t="s">
-        <v>127</v>
-      </c>
+      <c r="C43" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="50"/>
       <c r="E43" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F43" s="67"/>
-      <c r="G43" s="12"/>
+        <v>49</v>
+      </c>
+      <c r="F43" s="87"/>
+      <c r="G43" s="102" t="s">
+        <v>154</v>
+      </c>
       <c r="H43" s="37"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -2665,18 +2839,18 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="19"/>
       <c r="C44" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="51"/>
-      <c r="E44" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" s="68"/>
-      <c r="G44" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="D44" s="50"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G44" s="40"/>
       <c r="H44" s="37"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
@@ -2697,149 +2871,145 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A45" s="12"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="51"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
-    </row>
-    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="6"/>
-      <c r="T46" s="6"/>
-      <c r="U46" s="6"/>
-      <c r="V46" s="6"/>
-      <c r="W46" s="6"/>
-      <c r="X46" s="6"/>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6"/>
-    </row>
-    <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="69">
+    <row r="45" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="16"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
+    </row>
+    <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="67">
         <v>4</v>
       </c>
-      <c r="B47" s="72" t="s">
+      <c r="B46" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C46" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="75" t="s">
-        <v>128</v>
-      </c>
-      <c r="E47" s="29" t="s">
+      <c r="D46" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H46" s="37"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+    </row>
+    <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="68"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="88"/>
+      <c r="E47" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="G47" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H47" s="37"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-    </row>
-    <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="70"/>
-      <c r="B48" s="73"/>
-      <c r="C48" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="76"/>
-      <c r="E48" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="F48" s="67"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="9"/>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-      <c r="V48" s="9"/>
-      <c r="W48" s="9"/>
-      <c r="X48" s="9"/>
-      <c r="Y48" s="9"/>
-      <c r="Z48" s="9"/>
-    </row>
-    <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="70"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="21" t="s">
+      <c r="F47" s="86"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="9"/>
+    </row>
+    <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="68"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="76"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="67"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="92"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+    </row>
+    <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="68"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="93"/>
+      <c r="F49" s="86"/>
       <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="3"/>
@@ -2861,13 +3031,13 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="70"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="67"/>
+    <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="69"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="91"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="94"/>
+      <c r="F50" s="87"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="3"/>
@@ -2889,82 +3059,84 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="71"/>
-      <c r="B51" s="74"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-    </row>
-    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A52" s="16"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="6"/>
-      <c r="T52" s="6"/>
-      <c r="U52" s="6"/>
-      <c r="V52" s="6"/>
-      <c r="W52" s="6"/>
-      <c r="X52" s="6"/>
-      <c r="Y52" s="6"/>
-      <c r="Z52" s="6"/>
-    </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="46.8" customHeight="1">
-      <c r="A53" s="86">
+    <row r="51" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="16"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="6"/>
+      <c r="T51" s="6"/>
+      <c r="U51" s="6"/>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="6"/>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+    </row>
+    <row r="52" spans="1:26" s="4" customFormat="1" ht="46.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="74">
         <v>5</v>
       </c>
-      <c r="B53" s="85" t="s">
+      <c r="B52" s="73" t="s">
         <v>34</v>
       </c>
+      <c r="C52" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
+    </row>
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="74"/>
+      <c r="B53" s="73"/>
       <c r="C53" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="97" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="G53" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="D53" s="27"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="40"/>
       <c r="H53" s="37"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -2985,16 +3157,16 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="86"/>
-      <c r="B54" s="85"/>
+    <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="74"/>
+      <c r="B54" s="73"/>
       <c r="C54" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="90"/>
-      <c r="G54" s="40"/>
+      <c r="F54" s="66"/>
+      <c r="G54" s="12"/>
       <c r="H54" s="37"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -3015,82 +3187,81 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="86"/>
-      <c r="B55" s="85"/>
-      <c r="C55" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="91"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
-      <c r="Z55" s="3"/>
-    </row>
-    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="A56" s="16"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="6"/>
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
-      <c r="S56" s="6"/>
-      <c r="T56" s="6"/>
-      <c r="U56" s="6"/>
-      <c r="V56" s="6"/>
-      <c r="W56" s="6"/>
-      <c r="X56" s="6"/>
-      <c r="Y56" s="6"/>
-      <c r="Z56" s="6"/>
-    </row>
-    <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="86">
+    <row r="55" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="16"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="6"/>
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+      <c r="X55" s="6"/>
+      <c r="Y55" s="6"/>
+      <c r="Z55" s="6"/>
+    </row>
+    <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="74">
         <v>6</v>
       </c>
-      <c r="B57" s="85" t="s">
+      <c r="B56" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="95" t="s">
-        <v>130</v>
-      </c>
+      <c r="C56" s="23"/>
+      <c r="D56" s="75" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="12"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+    </row>
+    <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="74"/>
+      <c r="B57" s="73"/>
+      <c r="D57" s="75"/>
       <c r="E57" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="F57" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="G57" s="12"/>
+        <v>73</v>
+      </c>
+      <c r="F57" s="65"/>
+      <c r="G57" s="40"/>
       <c r="H57" s="37"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
@@ -3111,15 +3282,20 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="86"/>
-      <c r="B58" s="85"/>
-      <c r="D58" s="95"/>
+    <row r="58" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="74"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="76"/>
       <c r="E58" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F58" s="90"/>
-      <c r="G58" s="40"/>
+        <v>95</v>
+      </c>
+      <c r="F58" s="66"/>
+      <c r="G58" s="102" t="s">
+        <v>155</v>
+      </c>
       <c r="H58" s="37"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
@@ -3140,18 +3316,19 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="86"/>
-      <c r="B59" s="85"/>
-      <c r="C59" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D59" s="75"/>
-      <c r="E59" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="F59" s="91"/>
-      <c r="G59" s="40"/>
+    <row r="59" spans="1:26" s="8" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="48"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" s="40" t="s">
+        <v>156</v>
+      </c>
       <c r="H59" s="37"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
@@ -3172,18 +3349,19 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26" s="8" customFormat="1" ht="47.4" customHeight="1">
+    <row r="60" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="48"/>
       <c r="B60" s="47"/>
-      <c r="C60" s="51"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="28" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E60" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" s="50"/>
-      <c r="G60" s="40"/>
+        <v>108</v>
+      </c>
+      <c r="G60" s="40" t="s">
+        <v>136</v>
+      </c>
       <c r="H60" s="37"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
@@ -3204,86 +3382,84 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1">
-      <c r="A61" s="48"/>
-      <c r="B61" s="47"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="E61" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="F61" s="50"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-      <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
-      <c r="X61" s="3"/>
-      <c r="Y61" s="3"/>
-      <c r="Z61" s="3"/>
-    </row>
-    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.95" customHeight="1">
-      <c r="A62" s="16"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
-      <c r="N62" s="6"/>
-      <c r="O62" s="6"/>
-      <c r="P62" s="6"/>
-      <c r="Q62" s="6"/>
-      <c r="R62" s="6"/>
-      <c r="S62" s="6"/>
-      <c r="T62" s="6"/>
-      <c r="U62" s="6"/>
-      <c r="V62" s="6"/>
-      <c r="W62" s="6"/>
-      <c r="X62" s="6"/>
-      <c r="Y62" s="6"/>
-      <c r="Z62" s="6"/>
-    </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.95" customHeight="1">
-      <c r="A63" s="12">
+    <row r="61" spans="1:26" s="7" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="16"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+      <c r="W61" s="6"/>
+      <c r="X61" s="6"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="6"/>
+    </row>
+    <row r="62" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="67">
         <v>7</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B62" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C62" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="61"/>
+      <c r="D62" s="76"/>
+      <c r="E62" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="F62" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="G62" s="102" t="s">
+        <v>157</v>
+      </c>
+      <c r="H62" s="37"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3"/>
+    </row>
+    <row r="63" spans="1:26" s="8" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="69"/>
+      <c r="B63" s="72"/>
+      <c r="C63" s="91"/>
+      <c r="D63" s="89"/>
       <c r="E63" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="F63" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="G63" s="40" t="s">
-        <v>113</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="F63" s="87"/>
+      <c r="G63" s="102"/>
       <c r="H63" s="37"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
@@ -3304,7 +3480,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="18"/>
       <c r="C64" s="22"/>
@@ -3332,25 +3508,25 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="69">
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="67">
         <v>8</v>
       </c>
-      <c r="B65" s="72" t="s">
+      <c r="B65" s="70" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="61"/>
+      <c r="D65" s="57"/>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="66" t="s">
+      <c r="F65" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="40" t="s">
-        <v>114</v>
+      <c r="G65" s="102" t="s">
+        <v>160</v>
       </c>
       <c r="H65" s="37"/>
       <c r="I65" s="3"/>
@@ -3372,17 +3548,17 @@
       <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
     </row>
-    <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="70"/>
-      <c r="B66" s="73"/>
+    <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="68"/>
+      <c r="B66" s="71"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="61"/>
+      <c r="D66" s="57"/>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="90"/>
+      <c r="F66" s="65"/>
       <c r="G66" s="40"/>
       <c r="H66" s="37"/>
       <c r="I66" s="3"/>
@@ -3404,18 +3580,20 @@
       <c r="Y66" s="3"/>
       <c r="Z66" s="3"/>
     </row>
-    <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="70"/>
-      <c r="B67" s="73"/>
+    <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="68"/>
+      <c r="B67" s="71"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="61"/>
+      <c r="D67" s="57"/>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="90"/>
-      <c r="G67" s="12"/>
+      <c r="F67" s="65"/>
+      <c r="G67" s="40" t="s">
+        <v>161</v>
+      </c>
       <c r="H67" s="37"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
@@ -3436,13 +3614,13 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="71"/>
-      <c r="B68" s="74"/>
+    <row r="68" spans="1:26" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="69"/>
+      <c r="B68" s="72"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="61"/>
+      <c r="D68" s="57"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="91"/>
+      <c r="F68" s="66"/>
       <c r="G68" s="12"/>
       <c r="H68" s="37"/>
       <c r="I68" s="3"/>
@@ -3464,7 +3642,7 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16"/>
       <c r="B69" s="18"/>
       <c r="C69" s="22"/>
@@ -3492,7 +3670,7 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.2" customHeight="1">
+    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12">
         <v>9</v>
       </c>
@@ -3500,16 +3678,18 @@
         <v>50</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="98" t="s">
-        <v>133</v>
+      <c r="D70" s="63" t="s">
+        <v>127</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F70" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="G70" s="12"/>
+      <c r="G70" s="40" t="s">
+        <v>162</v>
+      </c>
       <c r="H70" s="37"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
@@ -3531,38 +3711,42 @@
       <c r="Z70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="E21:E24"/>
+  <mergeCells count="35">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F47:F51"/>
-    <mergeCell ref="F40:F44"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="F39:F43"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="E48:E50"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F11:F28"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
updated RTM , bug fixes and SRS
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="164">
   <si>
     <t>Project Name:</t>
   </si>
@@ -573,6 +573,9 @@
   <si>
     <t>CategoryPage.aspx</t>
   </si>
+  <si>
+    <t>DataAccessLayer.cs.validateUserNameDoesnotExist(string username)</t>
+  </si>
 </sst>
 </file>
 
@@ -581,7 +584,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,7 +859,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1033,14 +1036,41 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1060,49 +1090,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1126,29 +1114,41 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1477,11 +1477,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="23.25" style="17" customWidth="1"/>
     <col min="2" max="2" width="30.375" style="17" customWidth="1"/>
@@ -1494,25 +1494,25 @@
     <col min="9" max="16384" width="9.25" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="G1" s="43"/>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="95"/>
+      <c r="C2" s="90"/>
       <c r="D2" s="55" t="s">
         <v>51</v>
       </c>
@@ -1529,14 +1529,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="95"/>
+      <c r="C3" s="90"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1553,14 +1553,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A4" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="96">
+      <c r="B4" s="91">
         <v>43470</v>
       </c>
-      <c r="C4" s="96"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1577,10 +1577,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="42"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.15" customHeight="1">
       <c r="A6" s="42"/>
       <c r="B6" s="51"/>
       <c r="C6" s="52"/>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="H6" s="45"/>
     </row>
-    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1641,11 +1641,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="74">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
+      <c r="A8" s="93">
         <v>1</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="92" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1655,9 +1655,9 @@
       <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="77"/>
+      <c r="F8" s="94"/>
       <c r="G8" s="36"/>
-      <c r="H8" s="77"/>
+      <c r="H8" s="94"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1677,9 +1677,9 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="74"/>
-      <c r="B9" s="73"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
+      <c r="A9" s="93"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
@@ -1687,9 +1687,9 @@
       <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="77"/>
+      <c r="F9" s="94"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="77"/>
+      <c r="H9" s="94"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1709,7 +1709,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.9" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="18"/>
       <c r="C10" s="22"/>
@@ -1737,7 +1737,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
       <c r="A11" s="59">
         <v>2</v>
       </c>
@@ -1753,13 +1753,13 @@
       <c r="E11" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="95" t="s">
         <v>87</v>
       </c>
       <c r="G11" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="74"/>
+      <c r="H11" s="93"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1779,7 +1779,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
       <c r="A12" s="59"/>
       <c r="B12" s="58"/>
       <c r="C12" s="21" t="s">
@@ -1791,11 +1791,11 @@
       <c r="E12" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="79"/>
-      <c r="G12" s="103" t="s">
+      <c r="F12" s="96"/>
+      <c r="G12" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="74"/>
+      <c r="H12" s="93"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1815,7 +1815,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A13" s="59"/>
       <c r="B13" s="58"/>
       <c r="C13" s="21" t="s">
@@ -1827,8 +1827,10 @@
       <c r="E13" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="79"/>
-      <c r="G13" s="104"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="68" t="s">
+        <v>163</v>
+      </c>
       <c r="H13" s="37"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1849,7 +1851,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A14" s="59"/>
       <c r="B14" s="58"/>
       <c r="C14" s="21" t="s">
@@ -1861,7 +1863,7 @@
       <c r="E14" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="79"/>
+      <c r="F14" s="96"/>
       <c r="G14" s="20" t="s">
         <v>130</v>
       </c>
@@ -1885,7 +1887,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A15" s="59"/>
       <c r="B15" s="58"/>
       <c r="C15" s="21" t="s">
@@ -1897,7 +1899,7 @@
       <c r="E15" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="79"/>
+      <c r="F15" s="96"/>
       <c r="G15" s="20" t="s">
         <v>131</v>
       </c>
@@ -1921,7 +1923,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A16" s="59"/>
       <c r="B16" s="58"/>
       <c r="C16" s="23"/>
@@ -1931,7 +1933,7 @@
       <c r="E16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="79"/>
+      <c r="F16" s="96"/>
       <c r="G16" s="40" t="s">
         <v>132</v>
       </c>
@@ -1955,7 +1957,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A17" s="59"/>
       <c r="B17" s="58"/>
       <c r="C17" s="23"/>
@@ -1965,7 +1967,7 @@
       <c r="E17" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="79"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="40" t="s">
         <v>133</v>
       </c>
@@ -1989,7 +1991,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A18" s="59"/>
       <c r="B18" s="58"/>
       <c r="C18" s="23"/>
@@ -1999,7 +2001,7 @@
       <c r="E18" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="79"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="53" t="s">
         <v>128</v>
       </c>
@@ -2023,7 +2025,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A19" s="59"/>
       <c r="B19" s="58"/>
       <c r="C19" s="23"/>
@@ -2033,7 +2035,7 @@
       <c r="E19" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="79"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="40" t="s">
         <v>134</v>
       </c>
@@ -2057,7 +2059,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A20" s="59"/>
       <c r="B20" s="58"/>
       <c r="C20" s="23"/>
@@ -2067,7 +2069,7 @@
       <c r="E20" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="79"/>
+      <c r="F20" s="96"/>
       <c r="G20" s="40" t="s">
         <v>135</v>
       </c>
@@ -2091,7 +2093,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A21" s="59"/>
       <c r="B21" s="58"/>
       <c r="C21" s="23"/>
@@ -2099,7 +2101,7 @@
       <c r="E21" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="F21" s="79"/>
+      <c r="F21" s="96"/>
       <c r="G21" s="40" t="s">
         <v>136</v>
       </c>
@@ -2123,16 +2125,16 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A22" s="59"/>
       <c r="B22" s="58"/>
       <c r="C22" s="23"/>
       <c r="D22" s="56"/>
-      <c r="E22" s="80" t="s">
+      <c r="E22" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="79"/>
-      <c r="G22" s="97" t="s">
+      <c r="F22" s="96"/>
+      <c r="G22" s="99" t="s">
         <v>137</v>
       </c>
       <c r="H22" s="37"/>
@@ -2155,14 +2157,14 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A23" s="59"/>
       <c r="B23" s="58"/>
       <c r="C23" s="23"/>
       <c r="D23" s="56"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="98"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="100"/>
       <c r="H23" s="37"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -2183,7 +2185,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
       <c r="A24" s="59"/>
       <c r="B24" s="58"/>
       <c r="C24" s="23"/>
@@ -2191,8 +2193,8 @@
       <c r="E24" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="79"/>
-      <c r="G24" s="99" t="s">
+      <c r="F24" s="96"/>
+      <c r="G24" s="40" t="s">
         <v>137</v>
       </c>
       <c r="H24" s="37"/>
@@ -2215,7 +2217,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A25" s="59"/>
       <c r="B25" s="58"/>
       <c r="C25" s="23"/>
@@ -2223,8 +2225,8 @@
       <c r="E25" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="79"/>
-      <c r="G25" s="100" t="s">
+      <c r="F25" s="96"/>
+      <c r="G25" s="64" t="s">
         <v>138</v>
       </c>
       <c r="H25" s="37"/>
@@ -2247,7 +2249,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A26" s="59"/>
       <c r="B26" s="58"/>
       <c r="C26" s="23"/>
@@ -2255,7 +2257,7 @@
       <c r="E26" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="79"/>
+      <c r="F26" s="96"/>
       <c r="G26" s="40" t="s">
         <v>139</v>
       </c>
@@ -2279,7 +2281,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A27" s="59"/>
       <c r="B27" s="58"/>
       <c r="C27" s="23"/>
@@ -2287,7 +2289,7 @@
       <c r="E27" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="79"/>
+      <c r="F27" s="96"/>
       <c r="G27" s="40" t="s">
         <v>140</v>
       </c>
@@ -2311,7 +2313,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A28" s="59"/>
       <c r="B28" s="58"/>
       <c r="C28" s="23"/>
@@ -2319,7 +2321,7 @@
       <c r="E28" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="79"/>
+      <c r="F28" s="96"/>
       <c r="G28" s="40" t="s">
         <v>141</v>
       </c>
@@ -2343,7 +2345,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="19"/>
       <c r="C29" s="21"/>
@@ -2375,7 +2377,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" s="19"/>
       <c r="C30" s="21"/>
@@ -2407,7 +2409,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="19"/>
       <c r="C31" s="21"/>
@@ -2439,7 +2441,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A32" s="12"/>
       <c r="B32" s="19"/>
       <c r="C32" s="21"/>
@@ -2471,7 +2473,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A33" s="12"/>
       <c r="B33" s="19"/>
       <c r="C33" s="21"/>
@@ -2503,7 +2505,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A34" s="12"/>
       <c r="B34" s="19"/>
       <c r="C34" s="21"/>
@@ -2535,7 +2537,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="19"/>
       <c r="C35" s="21"/>
@@ -2567,7 +2569,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" s="8" customFormat="1" ht="24" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" s="19"/>
       <c r="C36" s="21"/>
@@ -2576,7 +2578,7 @@
         <v>70</v>
       </c>
       <c r="F36" s="33"/>
-      <c r="G36" s="100" t="s">
+      <c r="G36" s="64" t="s">
         <v>148</v>
       </c>
       <c r="H36" s="37"/>
@@ -2599,7 +2601,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="75.75" customHeight="1">
       <c r="A37" s="12"/>
       <c r="B37" s="19"/>
       <c r="C37" s="21"/>
@@ -2608,7 +2610,7 @@
         <v>97</v>
       </c>
       <c r="F37" s="33"/>
-      <c r="G37" s="101" t="s">
+      <c r="G37" s="65" t="s">
         <v>149</v>
       </c>
       <c r="H37" s="37"/>
@@ -2631,7 +2633,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1">
       <c r="A38" s="16"/>
       <c r="B38" s="18"/>
       <c r="C38" s="22"/>
@@ -2659,7 +2661,7 @@
       <c r="Y38" s="6"/>
       <c r="Z38" s="6"/>
     </row>
-    <row r="39" spans="1:26" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" s="8" customFormat="1" ht="57" customHeight="1">
       <c r="A39" s="12">
         <v>3</v>
       </c>
@@ -2675,10 +2677,10 @@
       <c r="E39" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="64" t="s">
+      <c r="F39" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="G39" s="102" t="s">
+      <c r="G39" s="66" t="s">
         <v>152</v>
       </c>
       <c r="H39" s="37"/>
@@ -2701,7 +2703,7 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A40" s="12"/>
       <c r="B40" s="19"/>
       <c r="C40" s="21" t="s">
@@ -2713,7 +2715,7 @@
       <c r="E40" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="86"/>
+      <c r="F40" s="74"/>
       <c r="G40" s="40" t="s">
         <v>153</v>
       </c>
@@ -2737,7 +2739,7 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1">
       <c r="A41" s="12"/>
       <c r="B41" s="19"/>
       <c r="C41" s="21" t="s">
@@ -2749,7 +2751,7 @@
       <c r="E41" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="86"/>
+      <c r="F41" s="74"/>
       <c r="G41" s="40" t="s">
         <v>153</v>
       </c>
@@ -2773,7 +2775,7 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" s="8" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" s="8" customFormat="1" ht="59.45" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" s="19"/>
       <c r="C42" s="21"/>
@@ -2783,7 +2785,7 @@
       <c r="E42" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="86"/>
+      <c r="F42" s="74"/>
       <c r="G42" s="40"/>
       <c r="H42" s="37"/>
       <c r="I42" s="3"/>
@@ -2805,7 +2807,7 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" s="8" customFormat="1" ht="46.5" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="19"/>
       <c r="C43" s="21" t="s">
@@ -2815,8 +2817,8 @@
       <c r="E43" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="87"/>
-      <c r="G43" s="102" t="s">
+      <c r="F43" s="75"/>
+      <c r="G43" s="66" t="s">
         <v>154</v>
       </c>
       <c r="H43" s="37"/>
@@ -2839,7 +2841,7 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A44" s="12"/>
       <c r="B44" s="19"/>
       <c r="C44" s="21" t="s">
@@ -2871,7 +2873,7 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
       <c r="A45" s="16"/>
       <c r="B45" s="18"/>
       <c r="C45" s="22"/>
@@ -2899,23 +2901,23 @@
       <c r="Y45" s="6"/>
       <c r="Z45" s="6"/>
     </row>
-    <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="67">
+    <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A46" s="76">
         <v>4</v>
       </c>
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="79" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="76" t="s">
+      <c r="D46" s="82" t="s">
         <v>122</v>
       </c>
       <c r="E46" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="64" t="s">
+      <c r="F46" s="73" t="s">
         <v>89</v>
       </c>
       <c r="G46" s="37" t="s">
@@ -2941,17 +2943,17 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="68"/>
-      <c r="B47" s="71"/>
+    <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A47" s="77"/>
+      <c r="B47" s="80"/>
       <c r="C47" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="88"/>
+      <c r="D47" s="83"/>
       <c r="E47" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="86"/>
+      <c r="F47" s="74"/>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
       <c r="I47" s="9"/>
@@ -2973,15 +2975,15 @@
       <c r="Y47" s="9"/>
       <c r="Z47" s="9"/>
     </row>
-    <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="68"/>
-      <c r="B48" s="71"/>
+    <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A48" s="77"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="88"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="86"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="74"/>
       <c r="G48" s="37"/>
       <c r="H48" s="37"/>
       <c r="I48" s="3"/>
@@ -3003,13 +3005,13 @@
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="68"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="88"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="86"/>
+    <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A49" s="77"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="88"/>
+      <c r="F49" s="74"/>
       <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="3"/>
@@ -3031,13 +3033,13 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="69"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="91"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="94"/>
-      <c r="F50" s="87"/>
+    <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A50" s="78"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="75"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="3"/>
@@ -3059,7 +3061,7 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
       <c r="A51" s="16"/>
       <c r="B51" s="18"/>
       <c r="C51" s="22"/>
@@ -3087,11 +3089,11 @@
       <c r="Y51" s="6"/>
       <c r="Z51" s="6"/>
     </row>
-    <row r="52" spans="1:26" s="4" customFormat="1" ht="46.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="74">
+    <row r="52" spans="1:26" s="4" customFormat="1" ht="46.9" customHeight="1">
+      <c r="A52" s="93">
         <v>5</v>
       </c>
-      <c r="B52" s="73" t="s">
+      <c r="B52" s="92" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -3103,7 +3105,7 @@
       <c r="E52" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F52" s="64" t="s">
+      <c r="F52" s="73" t="s">
         <v>90</v>
       </c>
       <c r="G52" s="12"/>
@@ -3127,15 +3129,15 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="74"/>
-      <c r="B53" s="73"/>
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A53" s="93"/>
+      <c r="B53" s="92"/>
       <c r="C53" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="27"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="65"/>
+      <c r="F53" s="97"/>
       <c r="G53" s="40"/>
       <c r="H53" s="37"/>
       <c r="I53" s="3"/>
@@ -3157,15 +3159,15 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="74"/>
-      <c r="B54" s="73"/>
+    <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A54" s="93"/>
+      <c r="B54" s="92"/>
       <c r="C54" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="66"/>
+      <c r="F54" s="98"/>
       <c r="G54" s="12"/>
       <c r="H54" s="37"/>
       <c r="I54" s="3"/>
@@ -3187,7 +3189,7 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
       <c r="A55" s="16"/>
       <c r="B55" s="18"/>
       <c r="C55" s="22"/>
@@ -3215,21 +3217,21 @@
       <c r="Y55" s="6"/>
       <c r="Z55" s="6"/>
     </row>
-    <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="74">
+    <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A56" s="93">
         <v>6</v>
       </c>
-      <c r="B56" s="73" t="s">
+      <c r="B56" s="92" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="23"/>
-      <c r="D56" s="75" t="s">
+      <c r="D56" s="103" t="s">
         <v>124</v>
       </c>
       <c r="E56" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F56" s="64" t="s">
+      <c r="F56" s="73" t="s">
         <v>92</v>
       </c>
       <c r="G56" s="12"/>
@@ -3253,14 +3255,14 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="74"/>
-      <c r="B57" s="73"/>
-      <c r="D57" s="75"/>
+    <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A57" s="93"/>
+      <c r="B57" s="92"/>
+      <c r="D57" s="103"/>
       <c r="E57" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="65"/>
+      <c r="F57" s="97"/>
       <c r="G57" s="40"/>
       <c r="H57" s="37"/>
       <c r="I57" s="3"/>
@@ -3282,18 +3284,18 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="74"/>
-      <c r="B58" s="73"/>
+    <row r="58" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
+      <c r="A58" s="93"/>
+      <c r="B58" s="92"/>
       <c r="C58" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="76"/>
+      <c r="D58" s="82"/>
       <c r="E58" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="F58" s="66"/>
-      <c r="G58" s="102" t="s">
+      <c r="F58" s="98"/>
+      <c r="G58" s="66" t="s">
         <v>155</v>
       </c>
       <c r="H58" s="37"/>
@@ -3316,7 +3318,7 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26" s="8" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" s="8" customFormat="1" ht="47.45" customHeight="1">
       <c r="A59" s="48"/>
       <c r="B59" s="47"/>
       <c r="C59" s="50"/>
@@ -3349,7 +3351,7 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1">
       <c r="A60" s="48"/>
       <c r="B60" s="47"/>
       <c r="C60" s="50"/>
@@ -3382,7 +3384,7 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="7" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" s="7" customFormat="1" ht="22.9" customHeight="1">
       <c r="A61" s="16"/>
       <c r="B61" s="18"/>
       <c r="C61" s="22"/>
@@ -3410,24 +3412,24 @@
       <c r="Y61" s="6"/>
       <c r="Z61" s="6"/>
     </row>
-    <row r="62" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="67">
+    <row r="62" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1">
+      <c r="A62" s="76">
         <v>7</v>
       </c>
-      <c r="B62" s="70" t="s">
+      <c r="B62" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="90" t="s">
+      <c r="C62" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="D62" s="76"/>
+      <c r="D62" s="82"/>
       <c r="E62" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="F62" s="64" t="s">
+      <c r="F62" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="G62" s="102" t="s">
+      <c r="G62" s="66" t="s">
         <v>157</v>
       </c>
       <c r="H62" s="37"/>
@@ -3450,16 +3452,16 @@
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
     </row>
-    <row r="63" spans="1:26" s="8" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="69"/>
-      <c r="B63" s="72"/>
-      <c r="C63" s="91"/>
-      <c r="D63" s="89"/>
+    <row r="63" spans="1:26" s="8" customFormat="1" ht="67.900000000000006" customHeight="1">
+      <c r="A63" s="78"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="84"/>
       <c r="E63" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="F63" s="87"/>
-      <c r="G63" s="102"/>
+      <c r="F63" s="75"/>
+      <c r="G63" s="66"/>
       <c r="H63" s="37"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
@@ -3480,7 +3482,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1">
       <c r="A64" s="16"/>
       <c r="B64" s="18"/>
       <c r="C64" s="22"/>
@@ -3508,11 +3510,11 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="67">
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="48.75" customHeight="1">
+      <c r="A65" s="76">
         <v>8</v>
       </c>
-      <c r="B65" s="70" t="s">
+      <c r="B65" s="79" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
@@ -3522,10 +3524,10 @@
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="64" t="s">
+      <c r="F65" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="102" t="s">
+      <c r="G65" s="66" t="s">
         <v>160</v>
       </c>
       <c r="H65" s="37"/>
@@ -3548,9 +3550,9 @@
       <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
     </row>
-    <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="68"/>
-      <c r="B66" s="71"/>
+    <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A66" s="77"/>
+      <c r="B66" s="80"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
@@ -3558,7 +3560,7 @@
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="65"/>
+      <c r="F66" s="97"/>
       <c r="G66" s="40"/>
       <c r="H66" s="37"/>
       <c r="I66" s="3"/>
@@ -3580,9 +3582,9 @@
       <c r="Y66" s="3"/>
       <c r="Z66" s="3"/>
     </row>
-    <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="68"/>
-      <c r="B67" s="71"/>
+    <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A67" s="77"/>
+      <c r="B67" s="80"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
@@ -3590,7 +3592,7 @@
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="65"/>
+      <c r="F67" s="97"/>
       <c r="G67" s="40" t="s">
         <v>161</v>
       </c>
@@ -3614,13 +3616,13 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="69"/>
-      <c r="B68" s="72"/>
+    <row r="68" spans="1:26" s="4" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A68" s="78"/>
+      <c r="B68" s="81"/>
       <c r="C68" s="21"/>
       <c r="D68" s="57"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="66"/>
+      <c r="F68" s="98"/>
       <c r="G68" s="12"/>
       <c r="H68" s="37"/>
       <c r="I68" s="3"/>
@@ -3642,7 +3644,7 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="A69" s="16"/>
       <c r="B69" s="18"/>
       <c r="C69" s="22"/>
@@ -3670,7 +3672,7 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.15" customHeight="1">
       <c r="A70" s="12">
         <v>9</v>
       </c>
@@ -3712,6 +3714,26 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F11:F28"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="E22:E23"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F46:F50"/>
@@ -3727,26 +3749,6 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F11:F28"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
committed test cases in RTM
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="175">
   <si>
     <t>Project Name:</t>
   </si>
@@ -575,6 +575,49 @@
   </si>
   <si>
     <t>DataAccessLayer.cs.validateUserNameDoesnotExist(string username)</t>
+  </si>
+  <si>
+    <t>RM_1</t>
+  </si>
+  <si>
+    <t>RM_3 , RM_4</t>
+  </si>
+  <si>
+    <t>RM_5 , RM_9 , RM_10 , RM_11 , RM_12 , RM_13</t>
+  </si>
+  <si>
+    <t>RM_6 , RM_7 , RM_14 , RM_15 , RM_16, RM_17 , RM_18 , RM_19 , RM_20 , RM_21</t>
+  </si>
+  <si>
+    <t>RM_8 , RM_22 , RM_23, RM_24 , RM_25</t>
+  </si>
+  <si>
+    <t>RM_2</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5 ,AM_6,AM_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat_Module_01
+Cat_Module_02
+Cat_Module_03
+Cat_Module_04
+Cat_Module_05
+</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5,AM_6,
+AM_7</t>
+  </si>
+  <si>
+    <t>AM_4 ,AM_8</t>
+  </si>
+  <si>
+    <t>AM_9</t>
   </si>
 </sst>
 </file>
@@ -859,7 +902,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -924,9 +967,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1015,40 +1055,112 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1063,46 +1175,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1114,40 +1190,13 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1477,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18"/>
@@ -1498,45 +1547,45 @@
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="43"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="101"/>
+      <c r="D2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="54" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="90"/>
+      <c r="C3" s="101"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1546,21 +1595,21 @@
       <c r="F3" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="44" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="102">
         <v>43470</v>
       </c>
-      <c r="C4" s="91"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1570,52 +1619,52 @@
       <c r="F4" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="44" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="72"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
       <c r="E5" s="14">
         <v>43601</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="44" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="2" customFormat="1" ht="55.15" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="13">
         <v>1.3</v>
       </c>
       <c r="E6" s="14">
         <v>43608</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="H6" s="45"/>
-    </row>
-    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1">
+      <c r="H6" s="44"/>
+    </row>
+    <row r="7" spans="1:26" s="43" customFormat="1" ht="93" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1642,22 +1691,22 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
-      <c r="A8" s="93">
+      <c r="A8" s="78">
         <v>1</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="77" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="29" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="94"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="94"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="85"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1678,18 +1727,18 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="93"/>
-      <c r="B9" s="92"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="29" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="94"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="94"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="85"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1738,28 +1787,28 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="59">
+      <c r="A11" s="57">
         <v>2</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="56" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="95" t="s">
+      <c r="F11" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="93"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1780,22 +1829,22 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="59"/>
-      <c r="B12" s="58"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="96"/>
-      <c r="G12" s="67" t="s">
+      <c r="F12" s="87"/>
+      <c r="G12" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="93"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1816,22 +1865,22 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="59"/>
-      <c r="B13" s="58"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="60" t="s">
+      <c r="E13" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="96"/>
-      <c r="G13" s="68" t="s">
+      <c r="F13" s="87"/>
+      <c r="G13" s="66" t="s">
         <v>163</v>
       </c>
-      <c r="H13" s="37"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1852,22 +1901,22 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="59"/>
-      <c r="B14" s="58"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="96"/>
+      <c r="F14" s="87"/>
       <c r="G14" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="37"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1888,22 +1937,22 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="59"/>
-      <c r="B15" s="58"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="96"/>
+      <c r="F15" s="87"/>
       <c r="G15" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H15" s="37"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1924,20 +1973,20 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="59"/>
-      <c r="B16" s="58"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="40" t="s">
+      <c r="F16" s="87"/>
+      <c r="G16" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="37"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1958,20 +2007,20 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="59"/>
-      <c r="B17" s="58"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="23"/>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="96"/>
-      <c r="G17" s="40" t="s">
+      <c r="F17" s="87"/>
+      <c r="G17" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="37"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1992,20 +2041,20 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="59"/>
-      <c r="B18" s="58"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="23"/>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="96"/>
-      <c r="G18" s="53" t="s">
+      <c r="F18" s="87"/>
+      <c r="G18" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2026,20 +2075,20 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="59"/>
-      <c r="B19" s="58"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="23"/>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="96"/>
-      <c r="G19" s="40" t="s">
+      <c r="F19" s="87"/>
+      <c r="G19" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="H19" s="37"/>
+      <c r="H19" s="36"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2060,20 +2109,20 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="59"/>
-      <c r="B20" s="58"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="23"/>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="96"/>
-      <c r="G20" s="40" t="s">
+      <c r="F20" s="87"/>
+      <c r="G20" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="37"/>
+      <c r="H20" s="36"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2094,18 +2143,18 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="59"/>
-      <c r="B21" s="58"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="23"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="60" t="s">
+      <c r="D21" s="55"/>
+      <c r="E21" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="F21" s="96"/>
-      <c r="G21" s="40" t="s">
+      <c r="F21" s="87"/>
+      <c r="G21" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="36"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2126,18 +2175,18 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="59"/>
-      <c r="B22" s="58"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="23"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="101" t="s">
+      <c r="D22" s="55"/>
+      <c r="E22" s="90" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="96"/>
-      <c r="G22" s="99" t="s">
+      <c r="F22" s="87"/>
+      <c r="G22" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="H22" s="37"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2158,14 +2207,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="58"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="37"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="36"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2186,18 +2235,20 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A24" s="59"/>
-      <c r="B24" s="58"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="23"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="60" t="s">
+      <c r="D24" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="96"/>
-      <c r="G24" s="40" t="s">
+      <c r="F24" s="87"/>
+      <c r="G24" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="37"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2218,18 +2269,18 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="59"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="60" t="s">
+      <c r="D25" s="97"/>
+      <c r="E25" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="96"/>
-      <c r="G25" s="64" t="s">
+      <c r="F25" s="87"/>
+      <c r="G25" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="H25" s="37"/>
+      <c r="H25" s="36"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2250,18 +2301,18 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="59"/>
-      <c r="B26" s="58"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="23"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="60" t="s">
+      <c r="D26" s="97"/>
+      <c r="E26" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="96"/>
-      <c r="G26" s="40" t="s">
+      <c r="F26" s="87"/>
+      <c r="G26" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="H26" s="37"/>
+      <c r="H26" s="36"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2282,18 +2333,18 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="59"/>
-      <c r="B27" s="58"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="23"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="60" t="s">
+      <c r="D27" s="97"/>
+      <c r="E27" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="96"/>
-      <c r="G27" s="40" t="s">
+      <c r="F27" s="87"/>
+      <c r="G27" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="H27" s="37"/>
+      <c r="H27" s="36"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2314,18 +2365,18 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="59"/>
-      <c r="B28" s="58"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="60" t="s">
+      <c r="D28" s="97"/>
+      <c r="E28" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="96"/>
-      <c r="G28" s="40" t="s">
+      <c r="F28" s="87"/>
+      <c r="G28" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="H28" s="37"/>
+      <c r="H28" s="36"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2349,15 +2400,15 @@
       <c r="A29" s="12"/>
       <c r="B29" s="19"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="60" t="s">
+      <c r="D29" s="97"/>
+      <c r="E29" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="40" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H29" s="37"/>
+      <c r="H29" s="36"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2381,15 +2432,15 @@
       <c r="A30" s="12"/>
       <c r="B30" s="19"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="60" t="s">
+      <c r="D30" s="97"/>
+      <c r="E30" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="40" t="s">
+      <c r="F30" s="32"/>
+      <c r="G30" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="H30" s="37"/>
+      <c r="H30" s="36"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2413,15 +2464,15 @@
       <c r="A31" s="12"/>
       <c r="B31" s="19"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="60" t="s">
+      <c r="D31" s="84"/>
+      <c r="E31" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="40" t="s">
+      <c r="F31" s="32"/>
+      <c r="G31" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="H31" s="37"/>
+      <c r="H31" s="36"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2441,19 +2492,21 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="32" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
       <c r="A32" s="12"/>
       <c r="B32" s="19"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="60" t="s">
+      <c r="D32" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="40" t="s">
+      <c r="F32" s="32"/>
+      <c r="G32" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="H32" s="37"/>
+      <c r="H32" s="36"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2473,19 +2526,21 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="33" spans="1:26" s="4" customFormat="1" ht="63" customHeight="1">
       <c r="A33" s="12"/>
       <c r="B33" s="19"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="60" t="s">
+      <c r="D33" s="103" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="40" t="s">
+      <c r="F33" s="32"/>
+      <c r="G33" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="H33" s="37"/>
+      <c r="H33" s="36"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2505,19 +2560,21 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="72.75" customHeight="1">
       <c r="A34" s="12"/>
       <c r="B34" s="19"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="60" t="s">
+      <c r="D34" s="80" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="33"/>
-      <c r="G34" s="40" t="s">
+      <c r="F34" s="32"/>
+      <c r="G34" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="H34" s="37"/>
+      <c r="H34" s="36"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2537,19 +2594,19 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="61.5" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="19"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="60" t="s">
+      <c r="D35" s="84"/>
+      <c r="E35" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="33"/>
-      <c r="G35" s="40" t="s">
+      <c r="F35" s="32"/>
+      <c r="G35" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="H35" s="37"/>
+      <c r="H35" s="36"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2569,19 +2626,21 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="8" customFormat="1" ht="24" customHeight="1">
+    <row r="36" spans="1:26" s="8" customFormat="1" ht="48.75" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" s="19"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="60" t="s">
+      <c r="D36" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="64" t="s">
+      <c r="F36" s="32"/>
+      <c r="G36" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="H36" s="37"/>
+      <c r="H36" s="36"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2605,15 +2664,17 @@
       <c r="A37" s="12"/>
       <c r="B37" s="19"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="60" t="s">
+      <c r="D37" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="33"/>
-      <c r="G37" s="65" t="s">
+      <c r="F37" s="32"/>
+      <c r="G37" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="H37" s="37"/>
+      <c r="H37" s="36"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2639,9 +2700,9 @@
       <c r="C38" s="22"/>
       <c r="D38" s="25"/>
       <c r="E38" s="18"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="41"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="40"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -2671,19 +2732,19 @@
       <c r="C39" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="61" t="s">
+      <c r="D39" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="73" t="s">
+      <c r="F39" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="G39" s="66" t="s">
+      <c r="G39" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="H39" s="37"/>
+      <c r="H39" s="36"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2709,17 +2770,17 @@
       <c r="C40" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="61" t="s">
+      <c r="D40" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="74"/>
-      <c r="G40" s="40" t="s">
+      <c r="F40" s="96"/>
+      <c r="G40" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="H40" s="37"/>
+      <c r="H40" s="36"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2745,17 +2806,17 @@
       <c r="C41" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="62" t="s">
+      <c r="D41" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="74"/>
-      <c r="G41" s="40" t="s">
+      <c r="F41" s="96"/>
+      <c r="G41" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="H41" s="37"/>
+      <c r="H41" s="36"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2779,15 +2840,15 @@
       <c r="A42" s="12"/>
       <c r="B42" s="19"/>
       <c r="C42" s="21"/>
-      <c r="D42" s="62" t="s">
+      <c r="D42" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="74"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="37"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="36"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2807,21 +2868,23 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="8" customFormat="1" ht="46.5" customHeight="1">
+    <row r="43" spans="1:26" s="8" customFormat="1" ht="78.75" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="19"/>
       <c r="C43" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D43" s="50"/>
-      <c r="E43" s="30" t="s">
+      <c r="D43" s="104" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="75"/>
-      <c r="G43" s="66" t="s">
+      <c r="F43" s="81"/>
+      <c r="G43" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="H43" s="37"/>
+      <c r="H43" s="36"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2841,19 +2904,19 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="44" spans="1:26" s="8" customFormat="1" ht="59.25" customHeight="1">
       <c r="A44" s="12"/>
       <c r="B44" s="19"/>
       <c r="C44" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="50"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="33" t="s">
+      <c r="D44" s="49"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G44" s="40"/>
-      <c r="H44" s="37"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2879,9 +2942,9 @@
       <c r="C45" s="22"/>
       <c r="D45" s="25"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="34"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="16"/>
-      <c r="H45" s="41"/>
+      <c r="H45" s="40"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -2902,28 +2965,28 @@
       <c r="Z45" s="6"/>
     </row>
     <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A46" s="76">
+      <c r="A46" s="71">
         <v>4</v>
       </c>
-      <c r="B46" s="79" t="s">
+      <c r="B46" s="74" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="82" t="s">
+      <c r="D46" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="29" t="s">
+      <c r="E46" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="73" t="s">
+      <c r="F46" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="37" t="s">
+      <c r="G46" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="H46" s="37"/>
+      <c r="H46" s="36"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -2944,18 +3007,18 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A47" s="77"/>
-      <c r="B47" s="80"/>
+      <c r="A47" s="72"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="83"/>
-      <c r="E47" s="31" t="s">
+      <c r="D47" s="97"/>
+      <c r="E47" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="74"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -2976,16 +3039,16 @@
       <c r="Z47" s="9"/>
     </row>
     <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A48" s="77"/>
-      <c r="B48" s="80"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="75"/>
       <c r="C48" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="83"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
+      <c r="D48" s="97"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -3006,14 +3069,14 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="77"/>
-      <c r="B49" s="80"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="88"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
+      <c r="A49" s="72"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="97"/>
+      <c r="E49" s="99"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -3034,14 +3097,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="78"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="86"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="83"/>
       <c r="D50" s="84"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
+      <c r="E50" s="100"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -3067,9 +3130,9 @@
       <c r="C51" s="22"/>
       <c r="D51" s="25"/>
       <c r="E51" s="18"/>
-      <c r="F51" s="34"/>
+      <c r="F51" s="33"/>
       <c r="G51" s="16"/>
-      <c r="H51" s="41"/>
+      <c r="H51" s="40"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -3090,26 +3153,26 @@
       <c r="Z51" s="6"/>
     </row>
     <row r="52" spans="1:26" s="4" customFormat="1" ht="46.9" customHeight="1">
-      <c r="A52" s="93">
+      <c r="A52" s="78">
         <v>5</v>
       </c>
-      <c r="B52" s="92" t="s">
+      <c r="B52" s="77" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="62" t="s">
+      <c r="D52" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="E52" s="29" t="s">
+      <c r="E52" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F52" s="73" t="s">
+      <c r="F52" s="68" t="s">
         <v>90</v>
       </c>
       <c r="G52" s="12"/>
-      <c r="H52" s="37"/>
+      <c r="H52" s="36"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -3130,16 +3193,16 @@
       <c r="Z52" s="3"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A53" s="93"/>
-      <c r="B53" s="92"/>
+      <c r="A53" s="78"/>
+      <c r="B53" s="77"/>
       <c r="C53" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="97"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="37"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="36"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -3160,16 +3223,16 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="93"/>
-      <c r="B54" s="92"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="77"/>
       <c r="C54" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="98"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="70"/>
       <c r="G54" s="12"/>
-      <c r="H54" s="37"/>
+      <c r="H54" s="36"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -3195,9 +3258,9 @@
       <c r="C55" s="22"/>
       <c r="D55" s="25"/>
       <c r="E55" s="18"/>
-      <c r="F55" s="34"/>
+      <c r="F55" s="33"/>
       <c r="G55" s="16"/>
-      <c r="H55" s="41"/>
+      <c r="H55" s="40"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -3218,24 +3281,24 @@
       <c r="Z55" s="6"/>
     </row>
     <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="93">
+      <c r="A56" s="78">
         <v>6</v>
       </c>
-      <c r="B56" s="92" t="s">
+      <c r="B56" s="77" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="23"/>
-      <c r="D56" s="103" t="s">
+      <c r="D56" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="E56" s="29" t="s">
+      <c r="E56" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F56" s="73" t="s">
+      <c r="F56" s="68" t="s">
         <v>92</v>
       </c>
       <c r="G56" s="12"/>
-      <c r="H56" s="37"/>
+      <c r="H56" s="36"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -3256,15 +3319,15 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A57" s="93"/>
-      <c r="B57" s="92"/>
-      <c r="D57" s="103"/>
-      <c r="E57" s="29" t="s">
+      <c r="A57" s="78"/>
+      <c r="B57" s="77"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="97"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="37"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="36"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3285,20 +3348,20 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A58" s="93"/>
-      <c r="B58" s="92"/>
+      <c r="A58" s="78"/>
+      <c r="B58" s="77"/>
       <c r="C58" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="82"/>
-      <c r="E58" s="29" t="s">
+      <c r="D58" s="80"/>
+      <c r="E58" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="F58" s="98"/>
-      <c r="G58" s="66" t="s">
+      <c r="F58" s="70"/>
+      <c r="G58" s="64" t="s">
         <v>155</v>
       </c>
-      <c r="H58" s="37"/>
+      <c r="H58" s="36"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3319,19 +3382,19 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="8" customFormat="1" ht="47.45" customHeight="1">
-      <c r="A59" s="48"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="28" t="s">
+      <c r="A59" s="47"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="49" t="s">
+      <c r="E59" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="G59" s="40" t="s">
+      <c r="G59" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="H59" s="37"/>
+      <c r="H59" s="36"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3352,19 +3415,19 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1">
-      <c r="A60" s="48"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="28" t="s">
+      <c r="A60" s="47"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="G60" s="40" t="s">
+      <c r="G60" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="H60" s="37"/>
+      <c r="H60" s="36"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3390,9 +3453,9 @@
       <c r="C61" s="22"/>
       <c r="D61" s="25"/>
       <c r="E61" s="18"/>
-      <c r="F61" s="34"/>
+      <c r="F61" s="33"/>
       <c r="G61" s="16"/>
-      <c r="H61" s="41"/>
+      <c r="H61" s="40"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3413,26 +3476,28 @@
       <c r="Z61" s="6"/>
     </row>
     <row r="62" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1">
-      <c r="A62" s="76">
+      <c r="A62" s="71">
         <v>7</v>
       </c>
-      <c r="B62" s="79" t="s">
+      <c r="B62" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="85" t="s">
+      <c r="C62" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="D62" s="82"/>
-      <c r="E62" s="32" t="s">
+      <c r="D62" s="80" t="s">
+        <v>171</v>
+      </c>
+      <c r="E62" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="F62" s="73" t="s">
+      <c r="F62" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="G62" s="66" t="s">
+      <c r="G62" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="H62" s="37"/>
+      <c r="H62" s="36"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -3453,16 +3518,16 @@
       <c r="Z62" s="3"/>
     </row>
     <row r="63" spans="1:26" s="8" customFormat="1" ht="67.900000000000006" customHeight="1">
-      <c r="A63" s="78"/>
-      <c r="B63" s="81"/>
-      <c r="C63" s="86"/>
+      <c r="A63" s="73"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="83"/>
       <c r="D63" s="84"/>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F63" s="75"/>
-      <c r="G63" s="66"/>
-      <c r="H63" s="37"/>
+      <c r="F63" s="81"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="36"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3488,9 +3553,9 @@
       <c r="C64" s="22"/>
       <c r="D64" s="25"/>
       <c r="E64" s="18"/>
-      <c r="F64" s="34"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="16"/>
-      <c r="H64" s="41"/>
+      <c r="H64" s="40"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3510,27 +3575,29 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="48.75" customHeight="1">
-      <c r="A65" s="76">
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="76.5" customHeight="1">
+      <c r="A65" s="71">
         <v>8</v>
       </c>
-      <c r="B65" s="79" t="s">
+      <c r="B65" s="74" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="57"/>
+      <c r="D65" s="105" t="s">
+        <v>172</v>
+      </c>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="73" t="s">
+      <c r="F65" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="66" t="s">
+      <c r="G65" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="H65" s="37"/>
+      <c r="H65" s="36"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3551,18 +3618,20 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="77"/>
-      <c r="B66" s="80"/>
+      <c r="A66" s="72"/>
+      <c r="B66" s="75"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="57"/>
+      <c r="D66" s="105" t="s">
+        <v>173</v>
+      </c>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="97"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="37"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="36"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -3583,20 +3652,22 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="77"/>
-      <c r="B67" s="80"/>
+      <c r="A67" s="72"/>
+      <c r="B67" s="75"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="57"/>
+      <c r="D67" s="105" t="s">
+        <v>174</v>
+      </c>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="97"/>
-      <c r="G67" s="40" t="s">
+      <c r="F67" s="69"/>
+      <c r="G67" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="H67" s="37"/>
+      <c r="H67" s="36"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -3617,14 +3688,14 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A68" s="78"/>
-      <c r="B68" s="81"/>
+      <c r="A68" s="73"/>
+      <c r="B68" s="76"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="57"/>
+      <c r="D68" s="67"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="98"/>
+      <c r="F68" s="70"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="37"/>
+      <c r="H68" s="36"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -3650,9 +3721,9 @@
       <c r="C69" s="22"/>
       <c r="D69" s="25"/>
       <c r="E69" s="18"/>
-      <c r="F69" s="34"/>
+      <c r="F69" s="33"/>
       <c r="G69" s="16"/>
-      <c r="H69" s="41"/>
+      <c r="H69" s="40"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -3680,19 +3751,19 @@
         <v>50</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="63" t="s">
+      <c r="D70" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="F70" s="35" t="s">
+      <c r="F70" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="G70" s="40" t="s">
+      <c r="G70" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="H70" s="37"/>
+      <c r="H70" s="36"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3713,27 +3784,7 @@
       <c r="Z70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F11:F28"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="E22:E23"/>
+  <mergeCells count="37">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F46:F50"/>
@@ -3749,6 +3800,28 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D24:D31"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F11:F28"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
minor updates in RTM
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_RTM.xlsx
+++ b/Requirements/Lhub_RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="171">
   <si>
     <t>Project Name:</t>
   </si>
@@ -475,9 +475,6 @@
     <t>LoginPage.aspx(passwordRequiredValidator)</t>
   </si>
   <si>
-    <t>LoginPage.aspx</t>
-  </si>
-  <si>
     <t>UserClass.cs.resetPassword(email,password)</t>
   </si>
   <si>
@@ -529,12 +526,6 @@
 , SignUpPage.aspx.emailRequiredValidator</t>
   </si>
   <si>
-    <t>Lhub_SRS_2.4.1.11</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.1.12</t>
-  </si>
-  <si>
     <t>HomePage.aspx.addBtn
 UploadArticlesPage.aspx</t>
   </si>
@@ -572,9 +563,6 @@
   </si>
   <si>
     <t>CategoryPage.aspx</t>
-  </si>
-  <si>
-    <t>DataAccessLayer.cs.validateUserNameDoesnotExist(string username)</t>
   </si>
   <si>
     <t>RM_1</t>
@@ -902,7 +890,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1085,20 +1073,38 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1117,68 +1123,20 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1190,13 +1148,40 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1526,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18"/>
@@ -1547,21 +1532,21 @@
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="101"/>
+      <c r="C2" s="91"/>
       <c r="D2" s="54" t="s">
         <v>51</v>
       </c>
@@ -1582,10 +1567,10 @@
       <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="101"/>
+      <c r="C3" s="91"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1606,10 +1591,10 @@
       <c r="A4" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="102">
+      <c r="B4" s="92">
         <v>43470</v>
       </c>
-      <c r="C4" s="102"/>
+      <c r="C4" s="92"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1628,8 +1613,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="41"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
@@ -1691,10 +1676,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
-      <c r="A8" s="78">
+      <c r="A8" s="94">
         <v>1</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="93" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1704,9 +1689,9 @@
       <c r="E8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="85"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="35"/>
-      <c r="H8" s="85"/>
+      <c r="H8" s="95"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1727,8 +1712,8 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="77"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
@@ -1736,9 +1721,9 @@
       <c r="E9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="85"/>
+      <c r="F9" s="95"/>
       <c r="G9" s="35"/>
-      <c r="H9" s="85"/>
+      <c r="H9" s="95"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1802,13 +1787,13 @@
       <c r="E11" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="86" t="s">
+      <c r="F11" s="96" t="s">
         <v>87</v>
       </c>
       <c r="G11" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="78"/>
+      <c r="H11" s="94"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1840,11 +1825,11 @@
       <c r="E12" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="87"/>
+      <c r="F12" s="97"/>
       <c r="G12" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="78"/>
+      <c r="H12" s="94"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1876,9 +1861,9 @@
       <c r="E13" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="66" t="s">
-        <v>163</v>
+      <c r="F13" s="97"/>
+      <c r="G13" s="20" t="s">
+        <v>130</v>
       </c>
       <c r="H13" s="36"/>
       <c r="I13" s="3"/>
@@ -1912,9 +1897,9 @@
       <c r="E14" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="87"/>
+      <c r="F14" s="97"/>
       <c r="G14" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H14" s="36"/>
       <c r="I14" s="3"/>
@@ -1948,9 +1933,9 @@
       <c r="E15" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="87"/>
-      <c r="G15" s="20" t="s">
-        <v>131</v>
+      <c r="F15" s="97"/>
+      <c r="G15" s="39" t="s">
+        <v>132</v>
       </c>
       <c r="H15" s="36"/>
       <c r="I15" s="3"/>
@@ -1982,9 +1967,9 @@
       <c r="E16" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="87"/>
-      <c r="G16" s="39" t="s">
-        <v>132</v>
+      <c r="F16" s="97"/>
+      <c r="G16" s="52" t="s">
+        <v>128</v>
       </c>
       <c r="H16" s="36"/>
       <c r="I16" s="3"/>
@@ -2016,7 +2001,7 @@
       <c r="E17" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="87"/>
+      <c r="F17" s="97"/>
       <c r="G17" s="39" t="s">
         <v>133</v>
       </c>
@@ -2050,9 +2035,9 @@
       <c r="E18" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="87"/>
-      <c r="G18" s="52" t="s">
-        <v>128</v>
+      <c r="F18" s="97"/>
+      <c r="G18" s="39" t="s">
+        <v>134</v>
       </c>
       <c r="H18" s="36"/>
       <c r="I18" s="3"/>
@@ -2084,7 +2069,7 @@
       <c r="E19" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="87"/>
+      <c r="F19" s="97"/>
       <c r="G19" s="39" t="s">
         <v>134</v>
       </c>
@@ -2118,9 +2103,9 @@
       <c r="E20" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="87"/>
-      <c r="G20" s="39" t="s">
-        <v>135</v>
+      <c r="F20" s="97"/>
+      <c r="G20" s="100" t="s">
+        <v>136</v>
       </c>
       <c r="H20" s="36"/>
       <c r="I20" s="3"/>
@@ -2142,18 +2127,14 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="21" spans="1:26" s="4" customFormat="1" ht="42" customHeight="1">
       <c r="A21" s="57"/>
       <c r="B21" s="56"/>
       <c r="C21" s="23"/>
       <c r="D21" s="55"/>
-      <c r="E21" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" s="87"/>
-      <c r="G21" s="39" t="s">
-        <v>136</v>
-      </c>
+      <c r="E21" s="58"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="101"/>
       <c r="H21" s="36"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -2179,13 +2160,8 @@
       <c r="B22" s="56"/>
       <c r="C22" s="23"/>
       <c r="D22" s="55"/>
-      <c r="E22" s="90" t="s">
-        <v>151</v>
-      </c>
-      <c r="F22" s="87"/>
-      <c r="G22" s="88" t="s">
-        <v>137</v>
-      </c>
+      <c r="E22" s="102"/>
+      <c r="F22" s="97"/>
       <c r="H22" s="36"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -2211,9 +2187,8 @@
       <c r="B23" s="56"/>
       <c r="C23" s="23"/>
       <c r="D23" s="55"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="89"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="97"/>
       <c r="H23" s="36"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -2238,15 +2213,15 @@
       <c r="A24" s="57"/>
       <c r="B24" s="56"/>
       <c r="C24" s="23"/>
-      <c r="D24" s="80" t="s">
-        <v>164</v>
+      <c r="D24" s="83" t="s">
+        <v>160</v>
       </c>
       <c r="E24" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="87"/>
+      <c r="F24" s="97"/>
       <c r="G24" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H24" s="36"/>
       <c r="I24" s="3"/>
@@ -2272,13 +2247,13 @@
       <c r="A25" s="57"/>
       <c r="B25" s="56"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="97"/>
+      <c r="D25" s="84"/>
       <c r="E25" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="87"/>
+      <c r="F25" s="97"/>
       <c r="G25" s="62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H25" s="36"/>
       <c r="I25" s="3"/>
@@ -2304,13 +2279,13 @@
       <c r="A26" s="57"/>
       <c r="B26" s="56"/>
       <c r="C26" s="23"/>
-      <c r="D26" s="97"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="87"/>
+      <c r="F26" s="97"/>
       <c r="G26" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H26" s="36"/>
       <c r="I26" s="3"/>
@@ -2336,13 +2311,13 @@
       <c r="A27" s="57"/>
       <c r="B27" s="56"/>
       <c r="C27" s="23"/>
-      <c r="D27" s="97"/>
+      <c r="D27" s="84"/>
       <c r="E27" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="87"/>
+      <c r="F27" s="97"/>
       <c r="G27" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H27" s="36"/>
       <c r="I27" s="3"/>
@@ -2368,13 +2343,13 @@
       <c r="A28" s="57"/>
       <c r="B28" s="56"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="97"/>
+      <c r="D28" s="84"/>
       <c r="E28" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="87"/>
+      <c r="F28" s="97"/>
       <c r="G28" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="3"/>
@@ -2400,13 +2375,13 @@
       <c r="A29" s="12"/>
       <c r="B29" s="19"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="97"/>
+      <c r="D29" s="84"/>
       <c r="E29" s="58" t="s">
         <v>63</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H29" s="36"/>
       <c r="I29" s="3"/>
@@ -2432,13 +2407,13 @@
       <c r="A30" s="12"/>
       <c r="B30" s="19"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="97"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="58" t="s">
         <v>64</v>
       </c>
       <c r="F30" s="32"/>
       <c r="G30" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H30" s="36"/>
       <c r="I30" s="3"/>
@@ -2464,13 +2439,13 @@
       <c r="A31" s="12"/>
       <c r="B31" s="19"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="84"/>
+      <c r="D31" s="85"/>
       <c r="E31" s="58" t="s">
         <v>65</v>
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H31" s="36"/>
       <c r="I31" s="3"/>
@@ -2496,15 +2471,15 @@
       <c r="A32" s="12"/>
       <c r="B32" s="19"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="67" t="s">
-        <v>165</v>
+      <c r="D32" s="66" t="s">
+        <v>161</v>
       </c>
       <c r="E32" s="58" t="s">
         <v>66</v>
       </c>
       <c r="F32" s="32"/>
       <c r="G32" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H32" s="36"/>
       <c r="I32" s="3"/>
@@ -2530,15 +2505,15 @@
       <c r="A33" s="12"/>
       <c r="B33" s="19"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="103" t="s">
-        <v>166</v>
+      <c r="D33" s="67" t="s">
+        <v>162</v>
       </c>
       <c r="E33" s="58" t="s">
         <v>67</v>
       </c>
       <c r="F33" s="32"/>
       <c r="G33" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H33" s="36"/>
       <c r="I33" s="3"/>
@@ -2564,15 +2539,15 @@
       <c r="A34" s="12"/>
       <c r="B34" s="19"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="80" t="s">
-        <v>167</v>
+      <c r="D34" s="83" t="s">
+        <v>163</v>
       </c>
       <c r="E34" s="58" t="s">
         <v>68</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H34" s="36"/>
       <c r="I34" s="3"/>
@@ -2598,13 +2573,13 @@
       <c r="A35" s="12"/>
       <c r="B35" s="19"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="84"/>
+      <c r="D35" s="85"/>
       <c r="E35" s="58" t="s">
         <v>69</v>
       </c>
       <c r="F35" s="32"/>
       <c r="G35" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H35" s="36"/>
       <c r="I35" s="3"/>
@@ -2630,15 +2605,15 @@
       <c r="A36" s="12"/>
       <c r="B36" s="19"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="67" t="s">
-        <v>168</v>
+      <c r="D36" s="66" t="s">
+        <v>164</v>
       </c>
       <c r="E36" s="58" t="s">
         <v>70</v>
       </c>
       <c r="F36" s="32"/>
       <c r="G36" s="62" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H36" s="36"/>
       <c r="I36" s="3"/>
@@ -2664,15 +2639,15 @@
       <c r="A37" s="12"/>
       <c r="B37" s="19"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="67" t="s">
-        <v>169</v>
+      <c r="D37" s="66" t="s">
+        <v>165</v>
       </c>
       <c r="E37" s="58" t="s">
         <v>97</v>
       </c>
       <c r="F37" s="32"/>
       <c r="G37" s="63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H37" s="36"/>
       <c r="I37" s="3"/>
@@ -2738,11 +2713,11 @@
       <c r="E39" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="68" t="s">
+      <c r="F39" s="74" t="s">
         <v>88</v>
       </c>
       <c r="G39" s="64" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H39" s="36"/>
       <c r="I39" s="3"/>
@@ -2776,9 +2751,9 @@
       <c r="E40" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="96"/>
+      <c r="F40" s="75"/>
       <c r="G40" s="39" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="3"/>
@@ -2812,9 +2787,9 @@
       <c r="E41" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="96"/>
+      <c r="F41" s="75"/>
       <c r="G41" s="39" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H41" s="36"/>
       <c r="I41" s="3"/>
@@ -2846,7 +2821,7 @@
       <c r="E42" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="96"/>
+      <c r="F42" s="75"/>
       <c r="G42" s="39"/>
       <c r="H42" s="36"/>
       <c r="I42" s="3"/>
@@ -2874,15 +2849,15 @@
       <c r="C43" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D43" s="104" t="s">
-        <v>170</v>
+      <c r="D43" s="68" t="s">
+        <v>166</v>
       </c>
       <c r="E43" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="81"/>
+      <c r="F43" s="76"/>
       <c r="G43" s="64" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H43" s="36"/>
       <c r="I43" s="3"/>
@@ -2965,22 +2940,22 @@
       <c r="Z45" s="6"/>
     </row>
     <row r="46" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A46" s="71">
+      <c r="A46" s="77">
         <v>4</v>
       </c>
-      <c r="B46" s="74" t="s">
+      <c r="B46" s="80" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="80" t="s">
+      <c r="D46" s="83" t="s">
         <v>122</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F46" s="68" t="s">
+      <c r="F46" s="74" t="s">
         <v>89</v>
       </c>
       <c r="G46" s="36" t="s">
@@ -3007,16 +2982,16 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A47" s="72"/>
-      <c r="B47" s="75"/>
+      <c r="A47" s="78"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="97"/>
+      <c r="D47" s="84"/>
       <c r="E47" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="96"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="37"/>
       <c r="H47" s="37"/>
       <c r="I47" s="9"/>
@@ -3039,14 +3014,14 @@
       <c r="Z47" s="9"/>
     </row>
     <row r="48" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A48" s="72"/>
-      <c r="B48" s="75"/>
+      <c r="A48" s="78"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="97"/>
-      <c r="E48" s="98"/>
-      <c r="F48" s="96"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="88"/>
+      <c r="F48" s="75"/>
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
       <c r="I48" s="3"/>
@@ -3069,12 +3044,12 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="72"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="97"/>
-      <c r="E49" s="99"/>
-      <c r="F49" s="96"/>
+      <c r="A49" s="78"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="75"/>
       <c r="G49" s="36"/>
       <c r="H49" s="36"/>
       <c r="I49" s="3"/>
@@ -3097,12 +3072,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="73"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="83"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="100"/>
-      <c r="F50" s="81"/>
+      <c r="A50" s="79"/>
+      <c r="B50" s="82"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="76"/>
       <c r="G50" s="36"/>
       <c r="H50" s="36"/>
       <c r="I50" s="3"/>
@@ -3153,10 +3128,10 @@
       <c r="Z51" s="6"/>
     </row>
     <row r="52" spans="1:26" s="4" customFormat="1" ht="46.9" customHeight="1">
-      <c r="A52" s="78">
+      <c r="A52" s="94">
         <v>5</v>
       </c>
-      <c r="B52" s="77" t="s">
+      <c r="B52" s="93" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -3168,7 +3143,7 @@
       <c r="E52" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F52" s="68" t="s">
+      <c r="F52" s="74" t="s">
         <v>90</v>
       </c>
       <c r="G52" s="12"/>
@@ -3193,14 +3168,14 @@
       <c r="Z52" s="3"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A53" s="78"/>
-      <c r="B53" s="77"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="93"/>
       <c r="C53" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="26"/>
       <c r="E53" s="28"/>
-      <c r="F53" s="69"/>
+      <c r="F53" s="98"/>
       <c r="G53" s="39"/>
       <c r="H53" s="36"/>
       <c r="I53" s="3"/>
@@ -3223,14 +3198,14 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="78"/>
-      <c r="B54" s="77"/>
+      <c r="A54" s="94"/>
+      <c r="B54" s="93"/>
       <c r="C54" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="28"/>
-      <c r="F54" s="70"/>
+      <c r="F54" s="99"/>
       <c r="G54" s="12"/>
       <c r="H54" s="36"/>
       <c r="I54" s="3"/>
@@ -3281,20 +3256,20 @@
       <c r="Z55" s="6"/>
     </row>
     <row r="56" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="78">
+      <c r="A56" s="94">
         <v>6</v>
       </c>
-      <c r="B56" s="77" t="s">
+      <c r="B56" s="93" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="23"/>
-      <c r="D56" s="79" t="s">
+      <c r="D56" s="104" t="s">
         <v>124</v>
       </c>
       <c r="E56" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F56" s="68" t="s">
+      <c r="F56" s="74" t="s">
         <v>92</v>
       </c>
       <c r="G56" s="12"/>
@@ -3319,13 +3294,13 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A57" s="78"/>
-      <c r="B57" s="77"/>
-      <c r="D57" s="79"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="93"/>
+      <c r="D57" s="104"/>
       <c r="E57" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="69"/>
+      <c r="F57" s="98"/>
       <c r="G57" s="39"/>
       <c r="H57" s="36"/>
       <c r="I57" s="3"/>
@@ -3348,18 +3323,18 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A58" s="78"/>
-      <c r="B58" s="77"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="93"/>
       <c r="C58" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="80"/>
+      <c r="D58" s="83"/>
       <c r="E58" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="F58" s="70"/>
+      <c r="F58" s="99"/>
       <c r="G58" s="64" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H58" s="36"/>
       <c r="I58" s="3"/>
@@ -3392,7 +3367,7 @@
         <v>96</v>
       </c>
       <c r="G59" s="39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H59" s="36"/>
       <c r="I59" s="3"/>
@@ -3425,7 +3400,7 @@
         <v>108</v>
       </c>
       <c r="G60" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H60" s="36"/>
       <c r="I60" s="3"/>
@@ -3476,26 +3451,26 @@
       <c r="Z61" s="6"/>
     </row>
     <row r="62" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1">
-      <c r="A62" s="71">
+      <c r="A62" s="77">
         <v>7</v>
       </c>
-      <c r="B62" s="74" t="s">
+      <c r="B62" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="82" t="s">
+      <c r="C62" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="D62" s="80" t="s">
-        <v>171</v>
+      <c r="D62" s="83" t="s">
+        <v>167</v>
       </c>
       <c r="E62" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="F62" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F62" s="74" t="s">
         <v>91</v>
       </c>
       <c r="G62" s="64" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H62" s="36"/>
       <c r="I62" s="3"/>
@@ -3518,14 +3493,14 @@
       <c r="Z62" s="3"/>
     </row>
     <row r="63" spans="1:26" s="8" customFormat="1" ht="67.900000000000006" customHeight="1">
-      <c r="A63" s="73"/>
-      <c r="B63" s="76"/>
-      <c r="C63" s="83"/>
-      <c r="D63" s="84"/>
+      <c r="A63" s="79"/>
+      <c r="B63" s="82"/>
+      <c r="C63" s="87"/>
+      <c r="D63" s="85"/>
       <c r="E63" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="F63" s="81"/>
+        <v>156</v>
+      </c>
+      <c r="F63" s="76"/>
       <c r="G63" s="64"/>
       <c r="H63" s="36"/>
       <c r="I63" s="3"/>
@@ -3576,26 +3551,26 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="76.5" customHeight="1">
-      <c r="A65" s="71">
+      <c r="A65" s="77">
         <v>8</v>
       </c>
-      <c r="B65" s="74" t="s">
+      <c r="B65" s="80" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="105" t="s">
-        <v>172</v>
+      <c r="D65" s="69" t="s">
+        <v>168</v>
       </c>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="68" t="s">
+      <c r="F65" s="74" t="s">
         <v>94</v>
       </c>
       <c r="G65" s="64" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H65" s="36"/>
       <c r="I65" s="3"/>
@@ -3618,18 +3593,18 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="72"/>
-      <c r="B66" s="75"/>
+      <c r="A66" s="78"/>
+      <c r="B66" s="81"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="105" t="s">
-        <v>173</v>
+      <c r="D66" s="69" t="s">
+        <v>169</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="69"/>
+      <c r="F66" s="98"/>
       <c r="G66" s="39"/>
       <c r="H66" s="36"/>
       <c r="I66" s="3"/>
@@ -3652,20 +3627,20 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="72"/>
-      <c r="B67" s="75"/>
+      <c r="A67" s="78"/>
+      <c r="B67" s="81"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="105" t="s">
-        <v>174</v>
+      <c r="D67" s="69" t="s">
+        <v>170</v>
       </c>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="69"/>
+      <c r="F67" s="98"/>
       <c r="G67" s="39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H67" s="36"/>
       <c r="I67" s="3"/>
@@ -3688,12 +3663,12 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A68" s="73"/>
-      <c r="B68" s="76"/>
+      <c r="A68" s="79"/>
+      <c r="B68" s="82"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="67"/>
+      <c r="D68" s="66"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="70"/>
+      <c r="F68" s="99"/>
       <c r="G68" s="12"/>
       <c r="H68" s="36"/>
       <c r="I68" s="3"/>
@@ -3761,7 +3736,7 @@
         <v>93</v>
       </c>
       <c r="G70" s="39" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H70" s="36"/>
       <c r="I70" s="3"/>
@@ -3785,6 +3760,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F11:F28"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F46:F50"/>
@@ -3801,27 +3797,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="D24:D31"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F11:F28"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>